<commit_message>
All data fully scraped as of today!
</commit_message>
<xml_diff>
--- a/Data/Odds/NFL/NFL odds 2021-22.xlsx
+++ b/Data/Odds/NFL/NFL odds 2021-22.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M33"/>
+  <dimension ref="A1:M127"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1946,6 +1946,4250 @@
         <v>24</v>
       </c>
     </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>916</v>
+      </c>
+      <c r="B34" t="n">
+        <v>101</v>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>NYGiants</t>
+        </is>
+      </c>
+      <c r="E34" t="n">
+        <v>7</v>
+      </c>
+      <c r="F34" t="n">
+        <v>3</v>
+      </c>
+      <c r="G34" t="n">
+        <v>10</v>
+      </c>
+      <c r="H34" t="n">
+        <v>9</v>
+      </c>
+      <c r="I34" t="n">
+        <v>29</v>
+      </c>
+      <c r="J34" t="n">
+        <v>42.5</v>
+      </c>
+      <c r="K34" t="n">
+        <v>41.5</v>
+      </c>
+      <c r="L34" t="n">
+        <v>175</v>
+      </c>
+      <c r="M34" t="n">
+        <v>20.5</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>916</v>
+      </c>
+      <c r="B35" t="n">
+        <v>102</v>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Washington</t>
+        </is>
+      </c>
+      <c r="E35" t="n">
+        <v>0</v>
+      </c>
+      <c r="F35" t="n">
+        <v>14</v>
+      </c>
+      <c r="G35" t="n">
+        <v>3</v>
+      </c>
+      <c r="H35" t="n">
+        <v>13</v>
+      </c>
+      <c r="I35" t="n">
+        <v>30</v>
+      </c>
+      <c r="J35" t="n">
+        <v>3</v>
+      </c>
+      <c r="K35" t="n">
+        <v>3</v>
+      </c>
+      <c r="L35" t="n">
+        <v>-200</v>
+      </c>
+      <c r="M35" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>919</v>
+      </c>
+      <c r="B36" t="n">
+        <v>269</v>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>NewOrleans</t>
+        </is>
+      </c>
+      <c r="E36" t="n">
+        <v>0</v>
+      </c>
+      <c r="F36" t="n">
+        <v>0</v>
+      </c>
+      <c r="G36" t="n">
+        <v>0</v>
+      </c>
+      <c r="H36" t="n">
+        <v>7</v>
+      </c>
+      <c r="I36" t="n">
+        <v>7</v>
+      </c>
+      <c r="J36" t="n">
+        <v>3</v>
+      </c>
+      <c r="K36" t="n">
+        <v>3</v>
+      </c>
+      <c r="L36" t="n">
+        <v>-150</v>
+      </c>
+      <c r="M36" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>919</v>
+      </c>
+      <c r="B37" t="n">
+        <v>270</v>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Carolina</t>
+        </is>
+      </c>
+      <c r="E37" t="n">
+        <v>7</v>
+      </c>
+      <c r="F37" t="n">
+        <v>10</v>
+      </c>
+      <c r="G37" t="n">
+        <v>0</v>
+      </c>
+      <c r="H37" t="n">
+        <v>9</v>
+      </c>
+      <c r="I37" t="n">
+        <v>26</v>
+      </c>
+      <c r="J37" t="n">
+        <v>46.5</v>
+      </c>
+      <c r="K37" t="n">
+        <v>45</v>
+      </c>
+      <c r="L37" t="n">
+        <v>130</v>
+      </c>
+      <c r="M37" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>919</v>
+      </c>
+      <c r="B38" t="n">
+        <v>271</v>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Houston</t>
+        </is>
+      </c>
+      <c r="E38" t="n">
+        <v>7</v>
+      </c>
+      <c r="F38" t="n">
+        <v>7</v>
+      </c>
+      <c r="G38" t="n">
+        <v>0</v>
+      </c>
+      <c r="H38" t="n">
+        <v>7</v>
+      </c>
+      <c r="I38" t="n">
+        <v>21</v>
+      </c>
+      <c r="J38" t="n">
+        <v>45.5</v>
+      </c>
+      <c r="K38" t="n">
+        <v>49</v>
+      </c>
+      <c r="L38" t="n">
+        <v>550</v>
+      </c>
+      <c r="M38" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>919</v>
+      </c>
+      <c r="B39" t="n">
+        <v>272</v>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Cleveland</t>
+        </is>
+      </c>
+      <c r="E39" t="n">
+        <v>7</v>
+      </c>
+      <c r="F39" t="n">
+        <v>7</v>
+      </c>
+      <c r="G39" t="n">
+        <v>10</v>
+      </c>
+      <c r="H39" t="n">
+        <v>7</v>
+      </c>
+      <c r="I39" t="n">
+        <v>31</v>
+      </c>
+      <c r="J39" t="n">
+        <v>13</v>
+      </c>
+      <c r="K39" t="n">
+        <v>14</v>
+      </c>
+      <c r="L39" t="n">
+        <v>-800</v>
+      </c>
+      <c r="M39" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>919</v>
+      </c>
+      <c r="B40" t="n">
+        <v>273</v>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Cincinnati</t>
+        </is>
+      </c>
+      <c r="E40" t="n">
+        <v>0</v>
+      </c>
+      <c r="F40" t="n">
+        <v>0</v>
+      </c>
+      <c r="G40" t="n">
+        <v>3</v>
+      </c>
+      <c r="H40" t="n">
+        <v>14</v>
+      </c>
+      <c r="I40" t="n">
+        <v>17</v>
+      </c>
+      <c r="J40" t="n">
+        <v>45.5</v>
+      </c>
+      <c r="K40" t="n">
+        <v>44.5</v>
+      </c>
+      <c r="L40" t="n">
+        <v>105</v>
+      </c>
+      <c r="M40" t="n">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>919</v>
+      </c>
+      <c r="B41" t="n">
+        <v>274</v>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Chicago</t>
+        </is>
+      </c>
+      <c r="E41" t="n">
+        <v>7</v>
+      </c>
+      <c r="F41" t="n">
+        <v>0</v>
+      </c>
+      <c r="G41" t="n">
+        <v>0</v>
+      </c>
+      <c r="H41" t="n">
+        <v>13</v>
+      </c>
+      <c r="I41" t="n">
+        <v>20</v>
+      </c>
+      <c r="J41" t="n">
+        <v>4</v>
+      </c>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>pk</t>
+        </is>
+      </c>
+      <c r="L41" t="n">
+        <v>-125</v>
+      </c>
+      <c r="M41" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>919</v>
+      </c>
+      <c r="B42" t="n">
+        <v>275</v>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>LasVegas</t>
+        </is>
+      </c>
+      <c r="E42" t="n">
+        <v>3</v>
+      </c>
+      <c r="F42" t="n">
+        <v>6</v>
+      </c>
+      <c r="G42" t="n">
+        <v>7</v>
+      </c>
+      <c r="H42" t="n">
+        <v>10</v>
+      </c>
+      <c r="I42" t="n">
+        <v>26</v>
+      </c>
+      <c r="J42" t="n">
+        <v>49.5</v>
+      </c>
+      <c r="K42" t="n">
+        <v>46.5</v>
+      </c>
+      <c r="L42" t="n">
+        <v>190</v>
+      </c>
+      <c r="M42" t="n">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>919</v>
+      </c>
+      <c r="B43" t="n">
+        <v>276</v>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Pittsburgh</t>
+        </is>
+      </c>
+      <c r="E43" t="n">
+        <v>0</v>
+      </c>
+      <c r="F43" t="n">
+        <v>7</v>
+      </c>
+      <c r="G43" t="n">
+        <v>0</v>
+      </c>
+      <c r="H43" t="n">
+        <v>10</v>
+      </c>
+      <c r="I43" t="n">
+        <v>17</v>
+      </c>
+      <c r="J43" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="K43" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="L43" t="n">
+        <v>-220</v>
+      </c>
+      <c r="M43" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>919</v>
+      </c>
+      <c r="B44" t="n">
+        <v>277</v>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>Buffalo</t>
+        </is>
+      </c>
+      <c r="E44" t="n">
+        <v>14</v>
+      </c>
+      <c r="F44" t="n">
+        <v>0</v>
+      </c>
+      <c r="G44" t="n">
+        <v>7</v>
+      </c>
+      <c r="H44" t="n">
+        <v>14</v>
+      </c>
+      <c r="I44" t="n">
+        <v>35</v>
+      </c>
+      <c r="J44" t="n">
+        <v>3</v>
+      </c>
+      <c r="K44" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="L44" t="n">
+        <v>-190</v>
+      </c>
+      <c r="M44" t="n">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>919</v>
+      </c>
+      <c r="B45" t="n">
+        <v>278</v>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Miami</t>
+        </is>
+      </c>
+      <c r="E45" t="n">
+        <v>0</v>
+      </c>
+      <c r="F45" t="n">
+        <v>0</v>
+      </c>
+      <c r="G45" t="n">
+        <v>0</v>
+      </c>
+      <c r="H45" t="n">
+        <v>0</v>
+      </c>
+      <c r="I45" t="n">
+        <v>0</v>
+      </c>
+      <c r="J45" t="n">
+        <v>48.5</v>
+      </c>
+      <c r="K45" t="n">
+        <v>48</v>
+      </c>
+      <c r="L45" t="n">
+        <v>170</v>
+      </c>
+      <c r="M45" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>919</v>
+      </c>
+      <c r="B46" t="n">
+        <v>279</v>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>LARams</t>
+        </is>
+      </c>
+      <c r="E46" t="n">
+        <v>7</v>
+      </c>
+      <c r="F46" t="n">
+        <v>3</v>
+      </c>
+      <c r="G46" t="n">
+        <v>7</v>
+      </c>
+      <c r="H46" t="n">
+        <v>10</v>
+      </c>
+      <c r="I46" t="n">
+        <v>27</v>
+      </c>
+      <c r="J46" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="K46" t="n">
+        <v>4</v>
+      </c>
+      <c r="L46" t="n">
+        <v>-210</v>
+      </c>
+      <c r="M46" t="n">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>919</v>
+      </c>
+      <c r="B47" t="n">
+        <v>280</v>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>Indianapolis</t>
+        </is>
+      </c>
+      <c r="E47" t="n">
+        <v>0</v>
+      </c>
+      <c r="F47" t="n">
+        <v>6</v>
+      </c>
+      <c r="G47" t="n">
+        <v>8</v>
+      </c>
+      <c r="H47" t="n">
+        <v>10</v>
+      </c>
+      <c r="I47" t="n">
+        <v>24</v>
+      </c>
+      <c r="J47" t="n">
+        <v>48.5</v>
+      </c>
+      <c r="K47" t="n">
+        <v>47.5</v>
+      </c>
+      <c r="L47" t="n">
+        <v>180</v>
+      </c>
+      <c r="M47" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>919</v>
+      </c>
+      <c r="B48" t="n">
+        <v>281</v>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>SanFrancisco</t>
+        </is>
+      </c>
+      <c r="E48" t="n">
+        <v>0</v>
+      </c>
+      <c r="F48" t="n">
+        <v>7</v>
+      </c>
+      <c r="G48" t="n">
+        <v>0</v>
+      </c>
+      <c r="H48" t="n">
+        <v>10</v>
+      </c>
+      <c r="I48" t="n">
+        <v>17</v>
+      </c>
+      <c r="J48" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="K48" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="L48" t="n">
+        <v>-150</v>
+      </c>
+      <c r="M48" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>919</v>
+      </c>
+      <c r="B49" t="n">
+        <v>282</v>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>Philadelphia</t>
+        </is>
+      </c>
+      <c r="E49" t="n">
+        <v>3</v>
+      </c>
+      <c r="F49" t="n">
+        <v>0</v>
+      </c>
+      <c r="G49" t="n">
+        <v>0</v>
+      </c>
+      <c r="H49" t="n">
+        <v>8</v>
+      </c>
+      <c r="I49" t="n">
+        <v>11</v>
+      </c>
+      <c r="J49" t="n">
+        <v>46.5</v>
+      </c>
+      <c r="K49" t="n">
+        <v>49</v>
+      </c>
+      <c r="L49" t="n">
+        <v>130</v>
+      </c>
+      <c r="M49" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>919</v>
+      </c>
+      <c r="B50" t="n">
+        <v>283</v>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>Denver</t>
+        </is>
+      </c>
+      <c r="E50" t="n">
+        <v>3</v>
+      </c>
+      <c r="F50" t="n">
+        <v>7</v>
+      </c>
+      <c r="G50" t="n">
+        <v>10</v>
+      </c>
+      <c r="H50" t="n">
+        <v>3</v>
+      </c>
+      <c r="I50" t="n">
+        <v>23</v>
+      </c>
+      <c r="J50" t="n">
+        <v>3</v>
+      </c>
+      <c r="K50" t="n">
+        <v>7</v>
+      </c>
+      <c r="L50" t="n">
+        <v>-260</v>
+      </c>
+      <c r="M50" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>919</v>
+      </c>
+      <c r="B51" t="n">
+        <v>284</v>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>Jacksonville</t>
+        </is>
+      </c>
+      <c r="E51" t="n">
+        <v>7</v>
+      </c>
+      <c r="F51" t="n">
+        <v>0</v>
+      </c>
+      <c r="G51" t="n">
+        <v>0</v>
+      </c>
+      <c r="H51" t="n">
+        <v>6</v>
+      </c>
+      <c r="I51" t="n">
+        <v>13</v>
+      </c>
+      <c r="J51" t="n">
+        <v>44.5</v>
+      </c>
+      <c r="K51" t="n">
+        <v>45</v>
+      </c>
+      <c r="L51" t="n">
+        <v>220</v>
+      </c>
+      <c r="M51" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>919</v>
+      </c>
+      <c r="B52" t="n">
+        <v>285</v>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>NewEngland</t>
+        </is>
+      </c>
+      <c r="E52" t="n">
+        <v>10</v>
+      </c>
+      <c r="F52" t="n">
+        <v>3</v>
+      </c>
+      <c r="G52" t="n">
+        <v>9</v>
+      </c>
+      <c r="H52" t="n">
+        <v>3</v>
+      </c>
+      <c r="I52" t="n">
+        <v>25</v>
+      </c>
+      <c r="J52" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="K52" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="L52" t="n">
+        <v>-240</v>
+      </c>
+      <c r="M52" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>919</v>
+      </c>
+      <c r="B53" t="n">
+        <v>286</v>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>NYJets</t>
+        </is>
+      </c>
+      <c r="E53" t="n">
+        <v>0</v>
+      </c>
+      <c r="F53" t="n">
+        <v>3</v>
+      </c>
+      <c r="G53" t="n">
+        <v>0</v>
+      </c>
+      <c r="H53" t="n">
+        <v>3</v>
+      </c>
+      <c r="I53" t="n">
+        <v>6</v>
+      </c>
+      <c r="J53" t="n">
+        <v>43.5</v>
+      </c>
+      <c r="K53" t="n">
+        <v>43</v>
+      </c>
+      <c r="L53" t="n">
+        <v>200</v>
+      </c>
+      <c r="M53" t="n">
+        <v>20.5</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>919</v>
+      </c>
+      <c r="B54" t="n">
+        <v>287</v>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>Minnesota</t>
+        </is>
+      </c>
+      <c r="E54" t="n">
+        <v>14</v>
+      </c>
+      <c r="F54" t="n">
+        <v>9</v>
+      </c>
+      <c r="G54" t="n">
+        <v>7</v>
+      </c>
+      <c r="H54" t="n">
+        <v>3</v>
+      </c>
+      <c r="I54" t="n">
+        <v>33</v>
+      </c>
+      <c r="J54" t="n">
+        <v>49.5</v>
+      </c>
+      <c r="K54" t="n">
+        <v>50.5</v>
+      </c>
+      <c r="L54" t="n">
+        <v>170</v>
+      </c>
+      <c r="M54" t="n">
+        <v>27.5</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>919</v>
+      </c>
+      <c r="B55" t="n">
+        <v>288</v>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>Arizona</t>
+        </is>
+      </c>
+      <c r="E55" t="n">
+        <v>7</v>
+      </c>
+      <c r="F55" t="n">
+        <v>17</v>
+      </c>
+      <c r="G55" t="n">
+        <v>7</v>
+      </c>
+      <c r="H55" t="n">
+        <v>3</v>
+      </c>
+      <c r="I55" t="n">
+        <v>34</v>
+      </c>
+      <c r="J55" t="n">
+        <v>3</v>
+      </c>
+      <c r="K55" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="L55" t="n">
+        <v>-190</v>
+      </c>
+      <c r="M55" t="n">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>919</v>
+      </c>
+      <c r="B56" t="n">
+        <v>289</v>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>Atlanta</t>
+        </is>
+      </c>
+      <c r="E56" t="n">
+        <v>0</v>
+      </c>
+      <c r="F56" t="n">
+        <v>10</v>
+      </c>
+      <c r="G56" t="n">
+        <v>15</v>
+      </c>
+      <c r="H56" t="n">
+        <v>0</v>
+      </c>
+      <c r="I56" t="n">
+        <v>25</v>
+      </c>
+      <c r="J56" t="n">
+        <v>52.5</v>
+      </c>
+      <c r="K56" t="n">
+        <v>52</v>
+      </c>
+      <c r="L56" t="n">
+        <v>550</v>
+      </c>
+      <c r="M56" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>919</v>
+      </c>
+      <c r="B57" t="n">
+        <v>290</v>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>TampaBay</t>
+        </is>
+      </c>
+      <c r="E57" t="n">
+        <v>7</v>
+      </c>
+      <c r="F57" t="n">
+        <v>14</v>
+      </c>
+      <c r="G57" t="n">
+        <v>7</v>
+      </c>
+      <c r="H57" t="n">
+        <v>20</v>
+      </c>
+      <c r="I57" t="n">
+        <v>48</v>
+      </c>
+      <c r="J57" t="n">
+        <v>9</v>
+      </c>
+      <c r="K57" t="n">
+        <v>14</v>
+      </c>
+      <c r="L57" t="n">
+        <v>-800</v>
+      </c>
+      <c r="M57" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>919</v>
+      </c>
+      <c r="B58" t="n">
+        <v>291</v>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>Tennessee</t>
+        </is>
+      </c>
+      <c r="E58" t="n">
+        <v>3</v>
+      </c>
+      <c r="F58" t="n">
+        <v>6</v>
+      </c>
+      <c r="G58" t="n">
+        <v>7</v>
+      </c>
+      <c r="H58" t="n">
+        <v>14</v>
+      </c>
+      <c r="I58" t="n">
+        <v>33</v>
+      </c>
+      <c r="J58" t="n">
+        <v>49.5</v>
+      </c>
+      <c r="K58" t="n">
+        <v>54</v>
+      </c>
+      <c r="L58" t="n">
+        <v>240</v>
+      </c>
+      <c r="M58" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>919</v>
+      </c>
+      <c r="B59" t="n">
+        <v>292</v>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>Seattle</t>
+        </is>
+      </c>
+      <c r="E59" t="n">
+        <v>3</v>
+      </c>
+      <c r="F59" t="n">
+        <v>21</v>
+      </c>
+      <c r="G59" t="n">
+        <v>0</v>
+      </c>
+      <c r="H59" t="n">
+        <v>6</v>
+      </c>
+      <c r="I59" t="n">
+        <v>30</v>
+      </c>
+      <c r="J59" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="K59" t="n">
+        <v>7</v>
+      </c>
+      <c r="L59" t="n">
+        <v>-280</v>
+      </c>
+      <c r="M59" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>919</v>
+      </c>
+      <c r="B60" t="n">
+        <v>293</v>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>Dallas</t>
+        </is>
+      </c>
+      <c r="E60" t="n">
+        <v>14</v>
+      </c>
+      <c r="F60" t="n">
+        <v>0</v>
+      </c>
+      <c r="G60" t="n">
+        <v>0</v>
+      </c>
+      <c r="H60" t="n">
+        <v>6</v>
+      </c>
+      <c r="I60" t="n">
+        <v>20</v>
+      </c>
+      <c r="J60" t="n">
+        <v>51.5</v>
+      </c>
+      <c r="K60" t="n">
+        <v>55</v>
+      </c>
+      <c r="L60" t="n">
+        <v>145</v>
+      </c>
+      <c r="M60" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>919</v>
+      </c>
+      <c r="B61" t="n">
+        <v>294</v>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>LAChargers</t>
+        </is>
+      </c>
+      <c r="E61" t="n">
+        <v>3</v>
+      </c>
+      <c r="F61" t="n">
+        <v>8</v>
+      </c>
+      <c r="G61" t="n">
+        <v>3</v>
+      </c>
+      <c r="H61" t="n">
+        <v>3</v>
+      </c>
+      <c r="I61" t="n">
+        <v>17</v>
+      </c>
+      <c r="J61" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="K61" t="n">
+        <v>3</v>
+      </c>
+      <c r="L61" t="n">
+        <v>-165</v>
+      </c>
+      <c r="M61" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>919</v>
+      </c>
+      <c r="B62" t="n">
+        <v>295</v>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>KansasCity</t>
+        </is>
+      </c>
+      <c r="E62" t="n">
+        <v>14</v>
+      </c>
+      <c r="F62" t="n">
+        <v>7</v>
+      </c>
+      <c r="G62" t="n">
+        <v>14</v>
+      </c>
+      <c r="H62" t="n">
+        <v>0</v>
+      </c>
+      <c r="I62" t="n">
+        <v>35</v>
+      </c>
+      <c r="J62" t="n">
+        <v>1</v>
+      </c>
+      <c r="K62" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="L62" t="n">
+        <v>-185</v>
+      </c>
+      <c r="M62" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>919</v>
+      </c>
+      <c r="B63" t="n">
+        <v>296</v>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>Baltimore</t>
+        </is>
+      </c>
+      <c r="E63" t="n">
+        <v>7</v>
+      </c>
+      <c r="F63" t="n">
+        <v>10</v>
+      </c>
+      <c r="G63" t="n">
+        <v>7</v>
+      </c>
+      <c r="H63" t="n">
+        <v>12</v>
+      </c>
+      <c r="I63" t="n">
+        <v>36</v>
+      </c>
+      <c r="J63" t="n">
+        <v>51.5</v>
+      </c>
+      <c r="K63" t="n">
+        <v>53.5</v>
+      </c>
+      <c r="L63" t="n">
+        <v>165</v>
+      </c>
+      <c r="M63" t="n">
+        <v>27.5</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>920</v>
+      </c>
+      <c r="B64" t="n">
+        <v>297</v>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>Detroit</t>
+        </is>
+      </c>
+      <c r="E64" t="n">
+        <v>7</v>
+      </c>
+      <c r="F64" t="n">
+        <v>10</v>
+      </c>
+      <c r="G64" t="n">
+        <v>0</v>
+      </c>
+      <c r="H64" t="n">
+        <v>0</v>
+      </c>
+      <c r="I64" t="n">
+        <v>17</v>
+      </c>
+      <c r="J64" t="n">
+        <v>48.5</v>
+      </c>
+      <c r="K64" t="n">
+        <v>49.5</v>
+      </c>
+      <c r="L64" t="n">
+        <v>450</v>
+      </c>
+      <c r="M64" t="n">
+        <v>26.5</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>920</v>
+      </c>
+      <c r="B65" t="n">
+        <v>298</v>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>GreenBay</t>
+        </is>
+      </c>
+      <c r="E65" t="n">
+        <v>7</v>
+      </c>
+      <c r="F65" t="n">
+        <v>7</v>
+      </c>
+      <c r="G65" t="n">
+        <v>14</v>
+      </c>
+      <c r="H65" t="n">
+        <v>7</v>
+      </c>
+      <c r="I65" t="n">
+        <v>35</v>
+      </c>
+      <c r="J65" t="n">
+        <v>7</v>
+      </c>
+      <c r="K65" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="L65" t="n">
+        <v>-600</v>
+      </c>
+      <c r="M65" t="n">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>923</v>
+      </c>
+      <c r="B66" t="n">
+        <v>301</v>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>Carolina</t>
+        </is>
+      </c>
+      <c r="E66" t="n">
+        <v>7</v>
+      </c>
+      <c r="F66" t="n">
+        <v>0</v>
+      </c>
+      <c r="G66" t="n">
+        <v>7</v>
+      </c>
+      <c r="H66" t="n">
+        <v>10</v>
+      </c>
+      <c r="I66" t="n">
+        <v>24</v>
+      </c>
+      <c r="J66" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="K66" t="n">
+        <v>9</v>
+      </c>
+      <c r="L66" t="n">
+        <v>-400</v>
+      </c>
+      <c r="M66" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>923</v>
+      </c>
+      <c r="B67" t="n">
+        <v>302</v>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>Houston</t>
+        </is>
+      </c>
+      <c r="E67" t="n">
+        <v>0</v>
+      </c>
+      <c r="F67" t="n">
+        <v>6</v>
+      </c>
+      <c r="G67" t="n">
+        <v>0</v>
+      </c>
+      <c r="H67" t="n">
+        <v>3</v>
+      </c>
+      <c r="I67" t="n">
+        <v>9</v>
+      </c>
+      <c r="J67" t="n">
+        <v>44.5</v>
+      </c>
+      <c r="K67" t="n">
+        <v>43</v>
+      </c>
+      <c r="L67" t="n">
+        <v>330</v>
+      </c>
+      <c r="M67" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>926</v>
+      </c>
+      <c r="B68" t="n">
+        <v>469</v>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>Arizona</t>
+        </is>
+      </c>
+      <c r="E68" t="n">
+        <v>7</v>
+      </c>
+      <c r="F68" t="n">
+        <v>0</v>
+      </c>
+      <c r="G68" t="n">
+        <v>17</v>
+      </c>
+      <c r="H68" t="n">
+        <v>7</v>
+      </c>
+      <c r="I68" t="n">
+        <v>31</v>
+      </c>
+      <c r="J68" t="n">
+        <v>6</v>
+      </c>
+      <c r="K68" t="n">
+        <v>9</v>
+      </c>
+      <c r="L68" t="n">
+        <v>-370</v>
+      </c>
+      <c r="M68" t="n">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>926</v>
+      </c>
+      <c r="B69" t="n">
+        <v>470</v>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>Jacksonville</t>
+        </is>
+      </c>
+      <c r="E69" t="n">
+        <v>0</v>
+      </c>
+      <c r="F69" t="n">
+        <v>13</v>
+      </c>
+      <c r="G69" t="n">
+        <v>6</v>
+      </c>
+      <c r="H69" t="n">
+        <v>0</v>
+      </c>
+      <c r="I69" t="n">
+        <v>19</v>
+      </c>
+      <c r="J69" t="n">
+        <v>50.5</v>
+      </c>
+      <c r="K69" t="n">
+        <v>51.5</v>
+      </c>
+      <c r="L69" t="n">
+        <v>310</v>
+      </c>
+      <c r="M69" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>926</v>
+      </c>
+      <c r="B70" t="n">
+        <v>471</v>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>Indianapolis</t>
+        </is>
+      </c>
+      <c r="E70" t="n">
+        <v>0</v>
+      </c>
+      <c r="F70" t="n">
+        <v>10</v>
+      </c>
+      <c r="G70" t="n">
+        <v>3</v>
+      </c>
+      <c r="H70" t="n">
+        <v>3</v>
+      </c>
+      <c r="I70" t="n">
+        <v>16</v>
+      </c>
+      <c r="J70" t="n">
+        <v>49.5</v>
+      </c>
+      <c r="K70" t="n">
+        <v>46.5</v>
+      </c>
+      <c r="L70" t="n">
+        <v>190</v>
+      </c>
+      <c r="M70" t="n">
+        <v>21.5</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>926</v>
+      </c>
+      <c r="B71" t="n">
+        <v>472</v>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>Tennessee</t>
+        </is>
+      </c>
+      <c r="E71" t="n">
+        <v>7</v>
+      </c>
+      <c r="F71" t="n">
+        <v>7</v>
+      </c>
+      <c r="G71" t="n">
+        <v>0</v>
+      </c>
+      <c r="H71" t="n">
+        <v>11</v>
+      </c>
+      <c r="I71" t="n">
+        <v>25</v>
+      </c>
+      <c r="J71" t="n">
+        <v>3</v>
+      </c>
+      <c r="K71" t="n">
+        <v>4</v>
+      </c>
+      <c r="L71" t="n">
+        <v>-220</v>
+      </c>
+      <c r="M71" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>926</v>
+      </c>
+      <c r="B72" t="n">
+        <v>473</v>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>Baltimore</t>
+        </is>
+      </c>
+      <c r="E72" t="n">
+        <v>0</v>
+      </c>
+      <c r="F72" t="n">
+        <v>10</v>
+      </c>
+      <c r="G72" t="n">
+        <v>6</v>
+      </c>
+      <c r="H72" t="n">
+        <v>3</v>
+      </c>
+      <c r="I72" t="n">
+        <v>19</v>
+      </c>
+      <c r="J72" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="K72" t="n">
+        <v>9</v>
+      </c>
+      <c r="L72" t="n">
+        <v>-360</v>
+      </c>
+      <c r="M72" t="n">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>926</v>
+      </c>
+      <c r="B73" t="n">
+        <v>474</v>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>Detroit</t>
+        </is>
+      </c>
+      <c r="E73" t="n">
+        <v>0</v>
+      </c>
+      <c r="F73" t="n">
+        <v>0</v>
+      </c>
+      <c r="G73" t="n">
+        <v>7</v>
+      </c>
+      <c r="H73" t="n">
+        <v>10</v>
+      </c>
+      <c r="I73" t="n">
+        <v>17</v>
+      </c>
+      <c r="J73" t="n">
+        <v>48.5</v>
+      </c>
+      <c r="K73" t="n">
+        <v>51</v>
+      </c>
+      <c r="L73" t="n">
+        <v>300</v>
+      </c>
+      <c r="M73" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>926</v>
+      </c>
+      <c r="B74" t="n">
+        <v>475</v>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>Washington</t>
+        </is>
+      </c>
+      <c r="E74" t="n">
+        <v>0</v>
+      </c>
+      <c r="F74" t="n">
+        <v>14</v>
+      </c>
+      <c r="G74" t="n">
+        <v>0</v>
+      </c>
+      <c r="H74" t="n">
+        <v>7</v>
+      </c>
+      <c r="I74" t="n">
+        <v>21</v>
+      </c>
+      <c r="J74" t="n">
+        <v>47.5</v>
+      </c>
+      <c r="K74" t="n">
+        <v>45.5</v>
+      </c>
+      <c r="L74" t="n">
+        <v>270</v>
+      </c>
+      <c r="M74" t="n">
+        <v>23.5</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>926</v>
+      </c>
+      <c r="B75" t="n">
+        <v>476</v>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>Buffalo</t>
+        </is>
+      </c>
+      <c r="E75" t="n">
+        <v>7</v>
+      </c>
+      <c r="F75" t="n">
+        <v>20</v>
+      </c>
+      <c r="G75" t="n">
+        <v>9</v>
+      </c>
+      <c r="H75" t="n">
+        <v>7</v>
+      </c>
+      <c r="I75" t="n">
+        <v>43</v>
+      </c>
+      <c r="J75" t="n">
+        <v>7</v>
+      </c>
+      <c r="K75" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="L75" t="n">
+        <v>-330</v>
+      </c>
+      <c r="M75" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>926</v>
+      </c>
+      <c r="B76" t="n">
+        <v>477</v>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>NewOrleans</t>
+        </is>
+      </c>
+      <c r="E76" t="n">
+        <v>7</v>
+      </c>
+      <c r="F76" t="n">
+        <v>7</v>
+      </c>
+      <c r="G76" t="n">
+        <v>7</v>
+      </c>
+      <c r="H76" t="n">
+        <v>7</v>
+      </c>
+      <c r="I76" t="n">
+        <v>28</v>
+      </c>
+      <c r="J76" t="n">
+        <v>46.5</v>
+      </c>
+      <c r="K76" t="n">
+        <v>43.5</v>
+      </c>
+      <c r="L76" t="n">
+        <v>130</v>
+      </c>
+      <c r="M76" t="n">
+        <v>20.5</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>926</v>
+      </c>
+      <c r="B77" t="n">
+        <v>478</v>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>NewEngland</t>
+        </is>
+      </c>
+      <c r="E77" t="n">
+        <v>0</v>
+      </c>
+      <c r="F77" t="n">
+        <v>3</v>
+      </c>
+      <c r="G77" t="n">
+        <v>3</v>
+      </c>
+      <c r="H77" t="n">
+        <v>7</v>
+      </c>
+      <c r="I77" t="n">
+        <v>13</v>
+      </c>
+      <c r="J77" t="inlineStr">
+        <is>
+          <t>pk</t>
+        </is>
+      </c>
+      <c r="K77" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="L77" t="n">
+        <v>-150</v>
+      </c>
+      <c r="M77" t="n">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>926</v>
+      </c>
+      <c r="B78" t="n">
+        <v>479</v>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>LAChargers</t>
+        </is>
+      </c>
+      <c r="E78" t="n">
+        <v>0</v>
+      </c>
+      <c r="F78" t="n">
+        <v>14</v>
+      </c>
+      <c r="G78" t="n">
+        <v>0</v>
+      </c>
+      <c r="H78" t="n">
+        <v>16</v>
+      </c>
+      <c r="I78" t="n">
+        <v>30</v>
+      </c>
+      <c r="J78" t="n">
+        <v>53</v>
+      </c>
+      <c r="K78" t="n">
+        <v>55</v>
+      </c>
+      <c r="L78" t="n">
+        <v>250</v>
+      </c>
+      <c r="M78" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>926</v>
+      </c>
+      <c r="B79" t="n">
+        <v>480</v>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>KansasCity</t>
+        </is>
+      </c>
+      <c r="E79" t="n">
+        <v>0</v>
+      </c>
+      <c r="F79" t="n">
+        <v>3</v>
+      </c>
+      <c r="G79" t="n">
+        <v>14</v>
+      </c>
+      <c r="H79" t="n">
+        <v>7</v>
+      </c>
+      <c r="I79" t="n">
+        <v>24</v>
+      </c>
+      <c r="J79" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="K79" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="L79" t="n">
+        <v>-300</v>
+      </c>
+      <c r="M79" t="n">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>926</v>
+      </c>
+      <c r="B80" t="n">
+        <v>481</v>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>Atlanta</t>
+        </is>
+      </c>
+      <c r="E80" t="n">
+        <v>0</v>
+      </c>
+      <c r="F80" t="n">
+        <v>7</v>
+      </c>
+      <c r="G80" t="n">
+        <v>0</v>
+      </c>
+      <c r="H80" t="n">
+        <v>10</v>
+      </c>
+      <c r="I80" t="n">
+        <v>17</v>
+      </c>
+      <c r="J80" t="n">
+        <v>43.5</v>
+      </c>
+      <c r="K80" t="n">
+        <v>47.5</v>
+      </c>
+      <c r="L80" t="n">
+        <v>130</v>
+      </c>
+      <c r="M80" t="n">
+        <v>22.5</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>926</v>
+      </c>
+      <c r="B81" t="n">
+        <v>482</v>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>NYGiants</t>
+        </is>
+      </c>
+      <c r="E81" t="n">
+        <v>3</v>
+      </c>
+      <c r="F81" t="n">
+        <v>3</v>
+      </c>
+      <c r="G81" t="n">
+        <v>0</v>
+      </c>
+      <c r="H81" t="n">
+        <v>8</v>
+      </c>
+      <c r="I81" t="n">
+        <v>14</v>
+      </c>
+      <c r="J81" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="K81" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="L81" t="n">
+        <v>-150</v>
+      </c>
+      <c r="M81" t="n">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>926</v>
+      </c>
+      <c r="B82" t="n">
+        <v>483</v>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>Chicago</t>
+        </is>
+      </c>
+      <c r="E82" t="n">
+        <v>3</v>
+      </c>
+      <c r="F82" t="n">
+        <v>0</v>
+      </c>
+      <c r="G82" t="n">
+        <v>3</v>
+      </c>
+      <c r="H82" t="n">
+        <v>0</v>
+      </c>
+      <c r="I82" t="n">
+        <v>6</v>
+      </c>
+      <c r="J82" t="n">
+        <v>46</v>
+      </c>
+      <c r="K82" t="n">
+        <v>44.5</v>
+      </c>
+      <c r="L82" t="n">
+        <v>310</v>
+      </c>
+      <c r="M82" t="n">
+        <v>21.5</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>926</v>
+      </c>
+      <c r="B83" t="n">
+        <v>484</v>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>Cleveland</t>
+        </is>
+      </c>
+      <c r="E83" t="n">
+        <v>0</v>
+      </c>
+      <c r="F83" t="n">
+        <v>10</v>
+      </c>
+      <c r="G83" t="n">
+        <v>3</v>
+      </c>
+      <c r="H83" t="n">
+        <v>13</v>
+      </c>
+      <c r="I83" t="n">
+        <v>26</v>
+      </c>
+      <c r="J83" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="K83" t="n">
+        <v>9</v>
+      </c>
+      <c r="L83" t="n">
+        <v>-370</v>
+      </c>
+      <c r="M83" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>926</v>
+      </c>
+      <c r="B84" t="n">
+        <v>485</v>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>Cincinnati</t>
+        </is>
+      </c>
+      <c r="E84" t="n">
+        <v>7</v>
+      </c>
+      <c r="F84" t="n">
+        <v>7</v>
+      </c>
+      <c r="G84" t="n">
+        <v>10</v>
+      </c>
+      <c r="H84" t="n">
+        <v>0</v>
+      </c>
+      <c r="I84" t="n">
+        <v>24</v>
+      </c>
+      <c r="J84" t="n">
+        <v>47.5</v>
+      </c>
+      <c r="K84" t="n">
+        <v>42</v>
+      </c>
+      <c r="L84" t="n">
+        <v>130</v>
+      </c>
+      <c r="M84" t="n">
+        <v>20.5</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>926</v>
+      </c>
+      <c r="B85" t="n">
+        <v>486</v>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>Pittsburgh</t>
+        </is>
+      </c>
+      <c r="E85" t="n">
+        <v>0</v>
+      </c>
+      <c r="F85" t="n">
+        <v>7</v>
+      </c>
+      <c r="G85" t="n">
+        <v>0</v>
+      </c>
+      <c r="H85" t="n">
+        <v>3</v>
+      </c>
+      <c r="I85" t="n">
+        <v>10</v>
+      </c>
+      <c r="J85" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="K85" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="L85" t="n">
+        <v>-150</v>
+      </c>
+      <c r="M85" t="n">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>926</v>
+      </c>
+      <c r="B86" t="n">
+        <v>487</v>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>Miami</t>
+        </is>
+      </c>
+      <c r="E86" t="n">
+        <v>14</v>
+      </c>
+      <c r="F86" t="n">
+        <v>0</v>
+      </c>
+      <c r="G86" t="n">
+        <v>0</v>
+      </c>
+      <c r="H86" t="n">
+        <v>11</v>
+      </c>
+      <c r="I86" t="n">
+        <v>28</v>
+      </c>
+      <c r="J86" t="n">
+        <v>48</v>
+      </c>
+      <c r="K86" t="n">
+        <v>45.5</v>
+      </c>
+      <c r="L86" t="n">
+        <v>170</v>
+      </c>
+      <c r="M86" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>926</v>
+      </c>
+      <c r="B87" t="n">
+        <v>488</v>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>LasVegas</t>
+        </is>
+      </c>
+      <c r="E87" t="n">
+        <v>2</v>
+      </c>
+      <c r="F87" t="n">
+        <v>10</v>
+      </c>
+      <c r="G87" t="n">
+        <v>7</v>
+      </c>
+      <c r="H87" t="n">
+        <v>6</v>
+      </c>
+      <c r="I87" t="n">
+        <v>31</v>
+      </c>
+      <c r="J87" t="n">
+        <v>1</v>
+      </c>
+      <c r="K87" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="L87" t="n">
+        <v>-190</v>
+      </c>
+      <c r="M87" t="n">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>926</v>
+      </c>
+      <c r="B88" t="n">
+        <v>489</v>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>NYJets</t>
+        </is>
+      </c>
+      <c r="E88" t="n">
+        <v>0</v>
+      </c>
+      <c r="F88" t="n">
+        <v>0</v>
+      </c>
+      <c r="G88" t="n">
+        <v>0</v>
+      </c>
+      <c r="H88" t="n">
+        <v>0</v>
+      </c>
+      <c r="I88" t="n">
+        <v>0</v>
+      </c>
+      <c r="J88" t="n">
+        <v>43.5</v>
+      </c>
+      <c r="K88" t="n">
+        <v>42</v>
+      </c>
+      <c r="L88" t="n">
+        <v>475</v>
+      </c>
+      <c r="M88" t="n">
+        <v>18.5</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>926</v>
+      </c>
+      <c r="B89" t="n">
+        <v>490</v>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>Denver</t>
+        </is>
+      </c>
+      <c r="E89" t="n">
+        <v>7</v>
+      </c>
+      <c r="F89" t="n">
+        <v>10</v>
+      </c>
+      <c r="G89" t="n">
+        <v>3</v>
+      </c>
+      <c r="H89" t="n">
+        <v>6</v>
+      </c>
+      <c r="I89" t="n">
+        <v>26</v>
+      </c>
+      <c r="J89" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="K89" t="n">
+        <v>11</v>
+      </c>
+      <c r="L89" t="n">
+        <v>-650</v>
+      </c>
+      <c r="M89" t="n">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>926</v>
+      </c>
+      <c r="B90" t="n">
+        <v>491</v>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>TampaBay</t>
+        </is>
+      </c>
+      <c r="E90" t="n">
+        <v>0</v>
+      </c>
+      <c r="F90" t="n">
+        <v>7</v>
+      </c>
+      <c r="G90" t="n">
+        <v>10</v>
+      </c>
+      <c r="H90" t="n">
+        <v>7</v>
+      </c>
+      <c r="I90" t="n">
+        <v>24</v>
+      </c>
+      <c r="J90" t="n">
+        <v>52.5</v>
+      </c>
+      <c r="K90" t="n">
+        <v>55</v>
+      </c>
+      <c r="L90" t="n">
+        <v>-105</v>
+      </c>
+      <c r="M90" t="n">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>926</v>
+      </c>
+      <c r="B91" t="n">
+        <v>492</v>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>LARams</t>
+        </is>
+      </c>
+      <c r="E91" t="n">
+        <v>0</v>
+      </c>
+      <c r="F91" t="n">
+        <v>14</v>
+      </c>
+      <c r="G91" t="n">
+        <v>17</v>
+      </c>
+      <c r="H91" t="n">
+        <v>3</v>
+      </c>
+      <c r="I91" t="n">
+        <v>34</v>
+      </c>
+      <c r="J91" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="K91" t="inlineStr">
+        <is>
+          <t>pk</t>
+        </is>
+      </c>
+      <c r="L91" t="n">
+        <v>-115</v>
+      </c>
+      <c r="M91" t="n">
+        <v>28.5</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>926</v>
+      </c>
+      <c r="B92" t="n">
+        <v>493</v>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>Seattle</t>
+        </is>
+      </c>
+      <c r="E92" t="n">
+        <v>10</v>
+      </c>
+      <c r="F92" t="n">
+        <v>7</v>
+      </c>
+      <c r="G92" t="n">
+        <v>0</v>
+      </c>
+      <c r="H92" t="n">
+        <v>0</v>
+      </c>
+      <c r="I92" t="n">
+        <v>17</v>
+      </c>
+      <c r="J92" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="K92" t="inlineStr">
+        <is>
+          <t>pk</t>
+        </is>
+      </c>
+      <c r="L92" t="n">
+        <v>-130</v>
+      </c>
+      <c r="M92" t="n">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>926</v>
+      </c>
+      <c r="B93" t="n">
+        <v>494</v>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>Minnesota</t>
+        </is>
+      </c>
+      <c r="E93" t="n">
+        <v>7</v>
+      </c>
+      <c r="F93" t="n">
+        <v>14</v>
+      </c>
+      <c r="G93" t="n">
+        <v>3</v>
+      </c>
+      <c r="H93" t="n">
+        <v>6</v>
+      </c>
+      <c r="I93" t="n">
+        <v>30</v>
+      </c>
+      <c r="J93" t="n">
+        <v>50.5</v>
+      </c>
+      <c r="K93" t="n">
+        <v>54</v>
+      </c>
+      <c r="L93" t="n">
+        <v>110</v>
+      </c>
+      <c r="M93" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>926</v>
+      </c>
+      <c r="B94" t="n">
+        <v>495</v>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>GreenBay</t>
+        </is>
+      </c>
+      <c r="E94" t="n">
+        <v>10</v>
+      </c>
+      <c r="F94" t="n">
+        <v>7</v>
+      </c>
+      <c r="G94" t="n">
+        <v>0</v>
+      </c>
+      <c r="H94" t="n">
+        <v>13</v>
+      </c>
+      <c r="I94" t="n">
+        <v>30</v>
+      </c>
+      <c r="J94" t="n">
+        <v>48</v>
+      </c>
+      <c r="K94" t="n">
+        <v>50.5</v>
+      </c>
+      <c r="L94" t="n">
+        <v>160</v>
+      </c>
+      <c r="M94" t="n">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>926</v>
+      </c>
+      <c r="B95" t="n">
+        <v>496</v>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>SanFrancisco</t>
+        </is>
+      </c>
+      <c r="E95" t="n">
+        <v>0</v>
+      </c>
+      <c r="F95" t="n">
+        <v>7</v>
+      </c>
+      <c r="G95" t="n">
+        <v>7</v>
+      </c>
+      <c r="H95" t="n">
+        <v>14</v>
+      </c>
+      <c r="I95" t="n">
+        <v>28</v>
+      </c>
+      <c r="J95" t="n">
+        <v>3</v>
+      </c>
+      <c r="K95" t="n">
+        <v>3</v>
+      </c>
+      <c r="L95" t="n">
+        <v>-180</v>
+      </c>
+      <c r="M95" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>927</v>
+      </c>
+      <c r="B96" t="n">
+        <v>497</v>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>Philadelphia</t>
+        </is>
+      </c>
+      <c r="E96" t="n">
+        <v>7</v>
+      </c>
+      <c r="F96" t="n">
+        <v>0</v>
+      </c>
+      <c r="G96" t="n">
+        <v>7</v>
+      </c>
+      <c r="H96" t="n">
+        <v>7</v>
+      </c>
+      <c r="I96" t="n">
+        <v>21</v>
+      </c>
+      <c r="J96" t="n">
+        <v>52.5</v>
+      </c>
+      <c r="K96" t="n">
+        <v>51.5</v>
+      </c>
+      <c r="L96" t="n">
+        <v>165</v>
+      </c>
+      <c r="M96" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>927</v>
+      </c>
+      <c r="B97" t="n">
+        <v>498</v>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>Dallas</t>
+        </is>
+      </c>
+      <c r="E97" t="n">
+        <v>14</v>
+      </c>
+      <c r="F97" t="n">
+        <v>6</v>
+      </c>
+      <c r="G97" t="n">
+        <v>7</v>
+      </c>
+      <c r="H97" t="n">
+        <v>14</v>
+      </c>
+      <c r="I97" t="n">
+        <v>41</v>
+      </c>
+      <c r="J97" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="K97" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="L97" t="n">
+        <v>-185</v>
+      </c>
+      <c r="M97" t="n">
+        <v>26.5</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>930</v>
+      </c>
+      <c r="B98" t="n">
+        <v>101</v>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>Jacksonville</t>
+        </is>
+      </c>
+      <c r="E98" t="n">
+        <v>7</v>
+      </c>
+      <c r="F98" t="n">
+        <v>7</v>
+      </c>
+      <c r="G98" t="n">
+        <v>0</v>
+      </c>
+      <c r="H98" t="n">
+        <v>7</v>
+      </c>
+      <c r="I98" t="n">
+        <v>21</v>
+      </c>
+      <c r="J98" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="K98" t="n">
+        <v>46</v>
+      </c>
+      <c r="L98" t="n">
+        <v>270</v>
+      </c>
+      <c r="M98" t="n">
+        <v>23.5</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>930</v>
+      </c>
+      <c r="B99" t="n">
+        <v>102</v>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>Cincinnati</t>
+        </is>
+      </c>
+      <c r="E99" t="n">
+        <v>0</v>
+      </c>
+      <c r="F99" t="n">
+        <v>0</v>
+      </c>
+      <c r="G99" t="n">
+        <v>14</v>
+      </c>
+      <c r="H99" t="n">
+        <v>10</v>
+      </c>
+      <c r="I99" t="n">
+        <v>24</v>
+      </c>
+      <c r="J99" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="K99" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="L99" t="n">
+        <v>-330</v>
+      </c>
+      <c r="M99" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>1003</v>
+      </c>
+      <c r="B100" t="n">
+        <v>251</v>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>Washington</t>
+        </is>
+      </c>
+      <c r="E100" t="n">
+        <v>0</v>
+      </c>
+      <c r="F100" t="n">
+        <v>13</v>
+      </c>
+      <c r="G100" t="n">
+        <v>9</v>
+      </c>
+      <c r="H100" t="n">
+        <v>12</v>
+      </c>
+      <c r="I100" t="n">
+        <v>34</v>
+      </c>
+      <c r="J100" t="n">
+        <v>1</v>
+      </c>
+      <c r="K100" t="inlineStr">
+        <is>
+          <t>pk</t>
+        </is>
+      </c>
+      <c r="L100" t="n">
+        <v>-125</v>
+      </c>
+      <c r="M100" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
+        <v>1003</v>
+      </c>
+      <c r="B101" t="n">
+        <v>252</v>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>Atlanta</t>
+        </is>
+      </c>
+      <c r="E101" t="n">
+        <v>3</v>
+      </c>
+      <c r="F101" t="n">
+        <v>14</v>
+      </c>
+      <c r="G101" t="n">
+        <v>6</v>
+      </c>
+      <c r="H101" t="n">
+        <v>7</v>
+      </c>
+      <c r="I101" t="n">
+        <v>30</v>
+      </c>
+      <c r="J101" t="n">
+        <v>49</v>
+      </c>
+      <c r="K101" t="n">
+        <v>46.5</v>
+      </c>
+      <c r="L101" t="n">
+        <v>105</v>
+      </c>
+      <c r="M101" t="n">
+        <v>23.5</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="n">
+        <v>1003</v>
+      </c>
+      <c r="B102" t="n">
+        <v>253</v>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>Detroit</t>
+        </is>
+      </c>
+      <c r="E102" t="n">
+        <v>0</v>
+      </c>
+      <c r="F102" t="n">
+        <v>0</v>
+      </c>
+      <c r="G102" t="n">
+        <v>7</v>
+      </c>
+      <c r="H102" t="n">
+        <v>7</v>
+      </c>
+      <c r="I102" t="n">
+        <v>14</v>
+      </c>
+      <c r="J102" t="n">
+        <v>45.5</v>
+      </c>
+      <c r="K102" t="n">
+        <v>41.5</v>
+      </c>
+      <c r="L102" t="n">
+        <v>130</v>
+      </c>
+      <c r="M102" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="n">
+        <v>1003</v>
+      </c>
+      <c r="B103" t="n">
+        <v>254</v>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>Chicago</t>
+        </is>
+      </c>
+      <c r="E103" t="n">
+        <v>7</v>
+      </c>
+      <c r="F103" t="n">
+        <v>7</v>
+      </c>
+      <c r="G103" t="n">
+        <v>10</v>
+      </c>
+      <c r="H103" t="n">
+        <v>0</v>
+      </c>
+      <c r="I103" t="n">
+        <v>24</v>
+      </c>
+      <c r="J103" t="n">
+        <v>6</v>
+      </c>
+      <c r="K103" t="n">
+        <v>3</v>
+      </c>
+      <c r="L103" t="n">
+        <v>-150</v>
+      </c>
+      <c r="M103" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="n">
+        <v>1003</v>
+      </c>
+      <c r="B104" t="n">
+        <v>255</v>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>Tennessee</t>
+        </is>
+      </c>
+      <c r="E104" t="n">
+        <v>3</v>
+      </c>
+      <c r="F104" t="n">
+        <v>6</v>
+      </c>
+      <c r="G104" t="n">
+        <v>0</v>
+      </c>
+      <c r="H104" t="n">
+        <v>15</v>
+      </c>
+      <c r="I104" t="n">
+        <v>24</v>
+      </c>
+      <c r="J104" t="n">
+        <v>6</v>
+      </c>
+      <c r="K104" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="L104" t="n">
+        <v>-250</v>
+      </c>
+      <c r="M104" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="n">
+        <v>1003</v>
+      </c>
+      <c r="B105" t="n">
+        <v>256</v>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>NY Jets</t>
+        </is>
+      </c>
+      <c r="E105" t="n">
+        <v>0</v>
+      </c>
+      <c r="F105" t="n">
+        <v>7</v>
+      </c>
+      <c r="G105" t="n">
+        <v>3</v>
+      </c>
+      <c r="H105" t="n">
+        <v>14</v>
+      </c>
+      <c r="I105" t="n">
+        <v>27</v>
+      </c>
+      <c r="J105" t="n">
+        <v>48.5</v>
+      </c>
+      <c r="K105" t="n">
+        <v>44</v>
+      </c>
+      <c r="L105" t="n">
+        <v>210</v>
+      </c>
+      <c r="M105" t="n">
+        <v>20.5</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="n">
+        <v>1003</v>
+      </c>
+      <c r="B106" t="n">
+        <v>257</v>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>Cleveland</t>
+        </is>
+      </c>
+      <c r="E106" t="n">
+        <v>0</v>
+      </c>
+      <c r="F106" t="n">
+        <v>11</v>
+      </c>
+      <c r="G106" t="n">
+        <v>0</v>
+      </c>
+      <c r="H106" t="n">
+        <v>3</v>
+      </c>
+      <c r="I106" t="n">
+        <v>14</v>
+      </c>
+      <c r="J106" t="n">
+        <v>1</v>
+      </c>
+      <c r="K106" t="n">
+        <v>52</v>
+      </c>
+      <c r="L106" t="n">
+        <v>-110</v>
+      </c>
+      <c r="M106" t="n">
+        <v>26.5</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="n">
+        <v>1003</v>
+      </c>
+      <c r="B107" t="n">
+        <v>258</v>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>Minnesota</t>
+        </is>
+      </c>
+      <c r="E107" t="n">
+        <v>7</v>
+      </c>
+      <c r="F107" t="n">
+        <v>0</v>
+      </c>
+      <c r="G107" t="n">
+        <v>0</v>
+      </c>
+      <c r="H107" t="n">
+        <v>0</v>
+      </c>
+      <c r="I107" t="n">
+        <v>7</v>
+      </c>
+      <c r="J107" t="n">
+        <v>50.5</v>
+      </c>
+      <c r="K107" t="inlineStr">
+        <is>
+          <t>pk</t>
+        </is>
+      </c>
+      <c r="L107" t="n">
+        <v>-110</v>
+      </c>
+      <c r="M107" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="n">
+        <v>1003</v>
+      </c>
+      <c r="B108" t="n">
+        <v>259</v>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>Indianapolis</t>
+        </is>
+      </c>
+      <c r="E108" t="n">
+        <v>0</v>
+      </c>
+      <c r="F108" t="n">
+        <v>7</v>
+      </c>
+      <c r="G108" t="n">
+        <v>10</v>
+      </c>
+      <c r="H108" t="n">
+        <v>10</v>
+      </c>
+      <c r="I108" t="n">
+        <v>27</v>
+      </c>
+      <c r="J108" t="n">
+        <v>45.5</v>
+      </c>
+      <c r="K108" t="n">
+        <v>42</v>
+      </c>
+      <c r="L108" t="n">
+        <v>130</v>
+      </c>
+      <c r="M108" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="n">
+        <v>1003</v>
+      </c>
+      <c r="B109" t="n">
+        <v>260</v>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>Miami</t>
+        </is>
+      </c>
+      <c r="E109" t="n">
+        <v>3</v>
+      </c>
+      <c r="F109" t="n">
+        <v>0</v>
+      </c>
+      <c r="G109" t="n">
+        <v>0</v>
+      </c>
+      <c r="H109" t="n">
+        <v>14</v>
+      </c>
+      <c r="I109" t="n">
+        <v>17</v>
+      </c>
+      <c r="J109" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="K109" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="L109" t="n">
+        <v>-150</v>
+      </c>
+      <c r="M109" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="n">
+        <v>1003</v>
+      </c>
+      <c r="B110" t="n">
+        <v>261</v>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>Carolina</t>
+        </is>
+      </c>
+      <c r="E110" t="n">
+        <v>7</v>
+      </c>
+      <c r="F110" t="n">
+        <v>7</v>
+      </c>
+      <c r="G110" t="n">
+        <v>0</v>
+      </c>
+      <c r="H110" t="n">
+        <v>14</v>
+      </c>
+      <c r="I110" t="n">
+        <v>28</v>
+      </c>
+      <c r="J110" t="n">
+        <v>50.5</v>
+      </c>
+      <c r="K110" t="n">
+        <v>51.5</v>
+      </c>
+      <c r="L110" t="n">
+        <v>185</v>
+      </c>
+      <c r="M110" t="n">
+        <v>26.5</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="n">
+        <v>1003</v>
+      </c>
+      <c r="B111" t="n">
+        <v>262</v>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>Dallas</t>
+        </is>
+      </c>
+      <c r="E111" t="n">
+        <v>7</v>
+      </c>
+      <c r="F111" t="n">
+        <v>6</v>
+      </c>
+      <c r="G111" t="n">
+        <v>20</v>
+      </c>
+      <c r="H111" t="n">
+        <v>3</v>
+      </c>
+      <c r="I111" t="n">
+        <v>36</v>
+      </c>
+      <c r="J111" t="n">
+        <v>4</v>
+      </c>
+      <c r="K111" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="L111" t="n">
+        <v>-215</v>
+      </c>
+      <c r="M111" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="n">
+        <v>1003</v>
+      </c>
+      <c r="B112" t="n">
+        <v>263</v>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>NY Giants</t>
+        </is>
+      </c>
+      <c r="E112" t="n">
+        <v>0</v>
+      </c>
+      <c r="F112" t="n">
+        <v>7</v>
+      </c>
+      <c r="G112" t="n">
+        <v>3</v>
+      </c>
+      <c r="H112" t="n">
+        <v>11</v>
+      </c>
+      <c r="I112" t="n">
+        <v>27</v>
+      </c>
+      <c r="J112" t="n">
+        <v>47</v>
+      </c>
+      <c r="K112" t="n">
+        <v>43</v>
+      </c>
+      <c r="L112" t="n">
+        <v>280</v>
+      </c>
+      <c r="M112" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="n">
+        <v>1003</v>
+      </c>
+      <c r="B113" t="n">
+        <v>264</v>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>New Orleans</t>
+        </is>
+      </c>
+      <c r="E113" t="n">
+        <v>0</v>
+      </c>
+      <c r="F113" t="n">
+        <v>7</v>
+      </c>
+      <c r="G113" t="n">
+        <v>7</v>
+      </c>
+      <c r="H113" t="n">
+        <v>7</v>
+      </c>
+      <c r="I113" t="n">
+        <v>21</v>
+      </c>
+      <c r="J113" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="K113" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="L113" t="n">
+        <v>-340</v>
+      </c>
+      <c r="M113" t="n">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="n">
+        <v>1003</v>
+      </c>
+      <c r="B114" t="n">
+        <v>265</v>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>Kansas City</t>
+        </is>
+      </c>
+      <c r="E114" t="n">
+        <v>7</v>
+      </c>
+      <c r="F114" t="n">
+        <v>14</v>
+      </c>
+      <c r="G114" t="n">
+        <v>7</v>
+      </c>
+      <c r="H114" t="n">
+        <v>14</v>
+      </c>
+      <c r="I114" t="n">
+        <v>42</v>
+      </c>
+      <c r="J114" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="K114" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="L114" t="n">
+        <v>-350</v>
+      </c>
+      <c r="M114" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="n">
+        <v>1003</v>
+      </c>
+      <c r="B115" t="n">
+        <v>266</v>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>Philadelphia</t>
+        </is>
+      </c>
+      <c r="E115" t="n">
+        <v>10</v>
+      </c>
+      <c r="F115" t="n">
+        <v>3</v>
+      </c>
+      <c r="G115" t="n">
+        <v>3</v>
+      </c>
+      <c r="H115" t="n">
+        <v>14</v>
+      </c>
+      <c r="I115" t="n">
+        <v>30</v>
+      </c>
+      <c r="J115" t="n">
+        <v>54.5</v>
+      </c>
+      <c r="K115" t="n">
+        <v>54</v>
+      </c>
+      <c r="L115" t="n">
+        <v>290</v>
+      </c>
+      <c r="M115" t="n">
+        <v>27.5</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="n">
+        <v>1003</v>
+      </c>
+      <c r="B116" t="n">
+        <v>267</v>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>Houston</t>
+        </is>
+      </c>
+      <c r="E116" t="n">
+        <v>0</v>
+      </c>
+      <c r="F116" t="n">
+        <v>0</v>
+      </c>
+      <c r="G116" t="n">
+        <v>0</v>
+      </c>
+      <c r="H116" t="n">
+        <v>0</v>
+      </c>
+      <c r="I116" t="n">
+        <v>0</v>
+      </c>
+      <c r="J116" t="n">
+        <v>48</v>
+      </c>
+      <c r="K116" t="n">
+        <v>47.5</v>
+      </c>
+      <c r="L116" t="n">
+        <v>1000</v>
+      </c>
+      <c r="M116" t="n">
+        <v>19.5</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="n">
+        <v>1003</v>
+      </c>
+      <c r="B117" t="n">
+        <v>268</v>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>Buffalo</t>
+        </is>
+      </c>
+      <c r="E117" t="n">
+        <v>7</v>
+      </c>
+      <c r="F117" t="n">
+        <v>9</v>
+      </c>
+      <c r="G117" t="n">
+        <v>3</v>
+      </c>
+      <c r="H117" t="n">
+        <v>21</v>
+      </c>
+      <c r="I117" t="n">
+        <v>40</v>
+      </c>
+      <c r="J117" t="n">
+        <v>16.5</v>
+      </c>
+      <c r="K117" t="n">
+        <v>18.5</v>
+      </c>
+      <c r="L117" t="n">
+        <v>-2000</v>
+      </c>
+      <c r="M117" t="n">
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="n">
+        <v>1003</v>
+      </c>
+      <c r="B118" t="n">
+        <v>269</v>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>Arizona</t>
+        </is>
+      </c>
+      <c r="E118" t="n">
+        <v>7</v>
+      </c>
+      <c r="F118" t="n">
+        <v>17</v>
+      </c>
+      <c r="G118" t="n">
+        <v>10</v>
+      </c>
+      <c r="H118" t="n">
+        <v>3</v>
+      </c>
+      <c r="I118" t="n">
+        <v>37</v>
+      </c>
+      <c r="J118" t="n">
+        <v>53</v>
+      </c>
+      <c r="K118" t="n">
+        <v>54</v>
+      </c>
+      <c r="L118" t="n">
+        <v>175</v>
+      </c>
+      <c r="M118" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="n">
+        <v>1003</v>
+      </c>
+      <c r="B119" t="n">
+        <v>270</v>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>LA Rams</t>
+        </is>
+      </c>
+      <c r="E119" t="n">
+        <v>10</v>
+      </c>
+      <c r="F119" t="n">
+        <v>3</v>
+      </c>
+      <c r="G119" t="n">
+        <v>0</v>
+      </c>
+      <c r="H119" t="n">
+        <v>7</v>
+      </c>
+      <c r="I119" t="n">
+        <v>20</v>
+      </c>
+      <c r="J119" t="n">
+        <v>6</v>
+      </c>
+      <c r="K119" t="n">
+        <v>4</v>
+      </c>
+      <c r="L119" t="n">
+        <v>-200</v>
+      </c>
+      <c r="M119" t="n">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="n">
+        <v>1003</v>
+      </c>
+      <c r="B120" t="n">
+        <v>271</v>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>Seattle</t>
+        </is>
+      </c>
+      <c r="E120" t="n">
+        <v>0</v>
+      </c>
+      <c r="F120" t="n">
+        <v>7</v>
+      </c>
+      <c r="G120" t="n">
+        <v>14</v>
+      </c>
+      <c r="H120" t="n">
+        <v>7</v>
+      </c>
+      <c r="I120" t="n">
+        <v>28</v>
+      </c>
+      <c r="J120" t="n">
+        <v>49.5</v>
+      </c>
+      <c r="K120" t="n">
+        <v>52</v>
+      </c>
+      <c r="L120" t="n">
+        <v>120</v>
+      </c>
+      <c r="M120" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="n">
+        <v>1003</v>
+      </c>
+      <c r="B121" t="n">
+        <v>272</v>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>San Francisco</t>
+        </is>
+      </c>
+      <c r="E121" t="n">
+        <v>7</v>
+      </c>
+      <c r="F121" t="n">
+        <v>0</v>
+      </c>
+      <c r="G121" t="n">
+        <v>6</v>
+      </c>
+      <c r="H121" t="n">
+        <v>8</v>
+      </c>
+      <c r="I121" t="n">
+        <v>21</v>
+      </c>
+      <c r="J121" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="K121" t="n">
+        <v>1</v>
+      </c>
+      <c r="L121" t="n">
+        <v>-140</v>
+      </c>
+      <c r="M121" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="n">
+        <v>1003</v>
+      </c>
+      <c r="B122" t="n">
+        <v>273</v>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>Baltimore</t>
+        </is>
+      </c>
+      <c r="E122" t="n">
+        <v>0</v>
+      </c>
+      <c r="F122" t="n">
+        <v>17</v>
+      </c>
+      <c r="G122" t="n">
+        <v>0</v>
+      </c>
+      <c r="H122" t="n">
+        <v>6</v>
+      </c>
+      <c r="I122" t="n">
+        <v>23</v>
+      </c>
+      <c r="J122" t="n">
+        <v>1</v>
+      </c>
+      <c r="K122" t="n">
+        <v>44</v>
+      </c>
+      <c r="L122" t="n">
+        <v>100</v>
+      </c>
+      <c r="M122" t="n">
+        <v>21.5</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="n">
+        <v>1003</v>
+      </c>
+      <c r="B123" t="n">
+        <v>274</v>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>Denver</t>
+        </is>
+      </c>
+      <c r="E123" t="n">
+        <v>0</v>
+      </c>
+      <c r="F123" t="n">
+        <v>7</v>
+      </c>
+      <c r="G123" t="n">
+        <v>0</v>
+      </c>
+      <c r="H123" t="n">
+        <v>0</v>
+      </c>
+      <c r="I123" t="n">
+        <v>7</v>
+      </c>
+      <c r="J123" t="n">
+        <v>45.5</v>
+      </c>
+      <c r="K123" t="inlineStr">
+        <is>
+          <t>pk</t>
+        </is>
+      </c>
+      <c r="L123" t="n">
+        <v>-120</v>
+      </c>
+      <c r="M123" t="n">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="n">
+        <v>1003</v>
+      </c>
+      <c r="B124" t="n">
+        <v>275</v>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>Pittsburgh</t>
+        </is>
+      </c>
+      <c r="E124" t="n">
+        <v>7</v>
+      </c>
+      <c r="F124" t="n">
+        <v>3</v>
+      </c>
+      <c r="G124" t="n">
+        <v>0</v>
+      </c>
+      <c r="H124" t="n">
+        <v>7</v>
+      </c>
+      <c r="I124" t="n">
+        <v>17</v>
+      </c>
+      <c r="J124" t="n">
+        <v>48</v>
+      </c>
+      <c r="K124" t="n">
+        <v>45</v>
+      </c>
+      <c r="L124" t="n">
+        <v>210</v>
+      </c>
+      <c r="M124" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="n">
+        <v>1003</v>
+      </c>
+      <c r="B125" t="n">
+        <v>276</v>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t>Green Bay</t>
+        </is>
+      </c>
+      <c r="E125" t="n">
+        <v>0</v>
+      </c>
+      <c r="F125" t="n">
+        <v>17</v>
+      </c>
+      <c r="G125" t="n">
+        <v>10</v>
+      </c>
+      <c r="H125" t="n">
+        <v>0</v>
+      </c>
+      <c r="I125" t="n">
+        <v>27</v>
+      </c>
+      <c r="J125" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="K125" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="L125" t="n">
+        <v>-250</v>
+      </c>
+      <c r="M125" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="n">
+        <v>1003</v>
+      </c>
+      <c r="B126" t="n">
+        <v>277</v>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t>Tampa Bay</t>
+        </is>
+      </c>
+      <c r="E126" t="n">
+        <v>3</v>
+      </c>
+      <c r="F126" t="n">
+        <v>3</v>
+      </c>
+      <c r="G126" t="n">
+        <v>7</v>
+      </c>
+      <c r="H126" t="n">
+        <v>6</v>
+      </c>
+      <c r="I126" t="n">
+        <v>19</v>
+      </c>
+      <c r="J126" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="K126" t="n">
+        <v>7</v>
+      </c>
+      <c r="L126" t="n">
+        <v>-300</v>
+      </c>
+      <c r="M126" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="n">
+        <v>1003</v>
+      </c>
+      <c r="B127" t="n">
+        <v>278</v>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D127" t="inlineStr">
+        <is>
+          <t>New England</t>
+        </is>
+      </c>
+      <c r="E127" t="n">
+        <v>0</v>
+      </c>
+      <c r="F127" t="n">
+        <v>7</v>
+      </c>
+      <c r="G127" t="n">
+        <v>0</v>
+      </c>
+      <c r="H127" t="n">
+        <v>10</v>
+      </c>
+      <c r="I127" t="n">
+        <v>17</v>
+      </c>
+      <c r="J127" t="n">
+        <v>50.5</v>
+      </c>
+      <c r="K127" t="n">
+        <v>49.5</v>
+      </c>
+      <c r="L127" t="n">
+        <v>250</v>
+      </c>
+      <c r="M127" t="n">
+        <v>23.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
modeling work, about to hack out esb scraper
</commit_message>
<xml_diff>
--- a/Data/Odds/NFL/NFL odds 2021-22.xlsx
+++ b/Data/Odds/NFL/NFL odds 2021-22.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M127"/>
+  <dimension ref="A1:M159"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6190,6 +6190,1448 @@
         <v>23.5</v>
       </c>
     </row>
+    <row r="128">
+      <c r="A128" t="n">
+        <v>1004</v>
+      </c>
+      <c r="B128" t="n">
+        <v>279</v>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D128" t="inlineStr">
+        <is>
+          <t>LasVegas</t>
+        </is>
+      </c>
+      <c r="E128" t="n">
+        <v>0</v>
+      </c>
+      <c r="F128" t="n">
+        <v>0</v>
+      </c>
+      <c r="G128" t="n">
+        <v>14</v>
+      </c>
+      <c r="H128" t="n">
+        <v>0</v>
+      </c>
+      <c r="I128" t="n">
+        <v>14</v>
+      </c>
+      <c r="J128" t="n">
+        <v>52.5</v>
+      </c>
+      <c r="K128" t="n">
+        <v>51.5</v>
+      </c>
+      <c r="L128" t="n">
+        <v>150</v>
+      </c>
+      <c r="M128" t="n">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="n">
+        <v>1004</v>
+      </c>
+      <c r="B129" t="n">
+        <v>280</v>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D129" t="inlineStr">
+        <is>
+          <t>LAChargers</t>
+        </is>
+      </c>
+      <c r="E129" t="n">
+        <v>7</v>
+      </c>
+      <c r="F129" t="n">
+        <v>14</v>
+      </c>
+      <c r="G129" t="n">
+        <v>0</v>
+      </c>
+      <c r="H129" t="n">
+        <v>7</v>
+      </c>
+      <c r="I129" t="n">
+        <v>28</v>
+      </c>
+      <c r="J129" t="n">
+        <v>3</v>
+      </c>
+      <c r="K129" t="n">
+        <v>3</v>
+      </c>
+      <c r="L129" t="n">
+        <v>-170</v>
+      </c>
+      <c r="M129" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="n">
+        <v>1007</v>
+      </c>
+      <c r="B130" t="n">
+        <v>301</v>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D130" t="inlineStr">
+        <is>
+          <t>LARams</t>
+        </is>
+      </c>
+      <c r="E130" t="n">
+        <v>0</v>
+      </c>
+      <c r="F130" t="n">
+        <v>3</v>
+      </c>
+      <c r="G130" t="n">
+        <v>13</v>
+      </c>
+      <c r="H130" t="n">
+        <v>10</v>
+      </c>
+      <c r="I130" t="n">
+        <v>26</v>
+      </c>
+      <c r="J130" t="n">
+        <v>52.5</v>
+      </c>
+      <c r="K130" t="n">
+        <v>3</v>
+      </c>
+      <c r="L130" t="n">
+        <v>-140</v>
+      </c>
+      <c r="M130" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="n">
+        <v>1007</v>
+      </c>
+      <c r="B131" t="n">
+        <v>302</v>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D131" t="inlineStr">
+        <is>
+          <t>Seattle</t>
+        </is>
+      </c>
+      <c r="E131" t="n">
+        <v>0</v>
+      </c>
+      <c r="F131" t="n">
+        <v>7</v>
+      </c>
+      <c r="G131" t="n">
+        <v>0</v>
+      </c>
+      <c r="H131" t="n">
+        <v>10</v>
+      </c>
+      <c r="I131" t="n">
+        <v>17</v>
+      </c>
+      <c r="J131" t="inlineStr">
+        <is>
+          <t>pk</t>
+        </is>
+      </c>
+      <c r="K131" t="n">
+        <v>53.5</v>
+      </c>
+      <c r="L131" t="n">
+        <v>120</v>
+      </c>
+      <c r="M131" t="n">
+        <v>26.5</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="n">
+        <v>1010</v>
+      </c>
+      <c r="B132" t="n">
+        <v>451</v>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D132" t="inlineStr">
+        <is>
+          <t>NYJets</t>
+        </is>
+      </c>
+      <c r="E132" t="n">
+        <v>0</v>
+      </c>
+      <c r="F132" t="n">
+        <v>3</v>
+      </c>
+      <c r="G132" t="n">
+        <v>6</v>
+      </c>
+      <c r="H132" t="n">
+        <v>11</v>
+      </c>
+      <c r="I132" t="n">
+        <v>20</v>
+      </c>
+      <c r="J132" t="n">
+        <v>44.5</v>
+      </c>
+      <c r="K132" t="n">
+        <v>45.5</v>
+      </c>
+      <c r="L132" t="n">
+        <v>130</v>
+      </c>
+      <c r="M132" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="n">
+        <v>1010</v>
+      </c>
+      <c r="B133" t="n">
+        <v>452</v>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D133" t="inlineStr">
+        <is>
+          <t>Atlanta</t>
+        </is>
+      </c>
+      <c r="E133" t="n">
+        <v>10</v>
+      </c>
+      <c r="F133" t="n">
+        <v>10</v>
+      </c>
+      <c r="G133" t="n">
+        <v>0</v>
+      </c>
+      <c r="H133" t="n">
+        <v>7</v>
+      </c>
+      <c r="I133" t="n">
+        <v>27</v>
+      </c>
+      <c r="J133" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="K133" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="L133" t="n">
+        <v>-150</v>
+      </c>
+      <c r="M133" t="n">
+        <v>22.5</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="n">
+        <v>1010</v>
+      </c>
+      <c r="B134" t="n">
+        <v>453</v>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D134" t="inlineStr">
+        <is>
+          <t>Miami</t>
+        </is>
+      </c>
+      <c r="E134" t="n">
+        <v>10</v>
+      </c>
+      <c r="F134" t="n">
+        <v>0</v>
+      </c>
+      <c r="G134" t="n">
+        <v>7</v>
+      </c>
+      <c r="H134" t="n">
+        <v>0</v>
+      </c>
+      <c r="I134" t="n">
+        <v>17</v>
+      </c>
+      <c r="J134" t="n">
+        <v>50</v>
+      </c>
+      <c r="K134" t="n">
+        <v>48</v>
+      </c>
+      <c r="L134" t="n">
+        <v>450</v>
+      </c>
+      <c r="M134" t="n">
+        <v>23.5</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="n">
+        <v>1010</v>
+      </c>
+      <c r="B135" t="n">
+        <v>454</v>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D135" t="inlineStr">
+        <is>
+          <t>TampaBay</t>
+        </is>
+      </c>
+      <c r="E135" t="n">
+        <v>7</v>
+      </c>
+      <c r="F135" t="n">
+        <v>17</v>
+      </c>
+      <c r="G135" t="n">
+        <v>0</v>
+      </c>
+      <c r="H135" t="n">
+        <v>21</v>
+      </c>
+      <c r="I135" t="n">
+        <v>45</v>
+      </c>
+      <c r="J135" t="n">
+        <v>9</v>
+      </c>
+      <c r="K135" t="n">
+        <v>12</v>
+      </c>
+      <c r="L135" t="n">
+        <v>-600</v>
+      </c>
+      <c r="M135" t="n">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="n">
+        <v>1010</v>
+      </c>
+      <c r="B136" t="n">
+        <v>455</v>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D136" t="inlineStr">
+        <is>
+          <t>Philadelphia</t>
+        </is>
+      </c>
+      <c r="E136" t="n">
+        <v>3</v>
+      </c>
+      <c r="F136" t="n">
+        <v>3</v>
+      </c>
+      <c r="G136" t="n">
+        <v>7</v>
+      </c>
+      <c r="H136" t="n">
+        <v>8</v>
+      </c>
+      <c r="I136" t="n">
+        <v>21</v>
+      </c>
+      <c r="J136" t="n">
+        <v>47</v>
+      </c>
+      <c r="K136" t="n">
+        <v>46.5</v>
+      </c>
+      <c r="L136" t="n">
+        <v>120</v>
+      </c>
+      <c r="M136" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="n">
+        <v>1010</v>
+      </c>
+      <c r="B137" t="n">
+        <v>456</v>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D137" t="inlineStr">
+        <is>
+          <t>Carolina</t>
+        </is>
+      </c>
+      <c r="E137" t="n">
+        <v>10</v>
+      </c>
+      <c r="F137" t="n">
+        <v>5</v>
+      </c>
+      <c r="G137" t="n">
+        <v>0</v>
+      </c>
+      <c r="H137" t="n">
+        <v>3</v>
+      </c>
+      <c r="I137" t="n">
+        <v>18</v>
+      </c>
+      <c r="J137" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="K137" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="L137" t="n">
+        <v>-140</v>
+      </c>
+      <c r="M137" t="n">
+        <v>21.5</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="n">
+        <v>1010</v>
+      </c>
+      <c r="B138" t="n">
+        <v>457</v>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D138" t="inlineStr">
+        <is>
+          <t>NewOrleans</t>
+        </is>
+      </c>
+      <c r="E138" t="n">
+        <v>7</v>
+      </c>
+      <c r="F138" t="n">
+        <v>13</v>
+      </c>
+      <c r="G138" t="n">
+        <v>0</v>
+      </c>
+      <c r="H138" t="n">
+        <v>13</v>
+      </c>
+      <c r="I138" t="n">
+        <v>33</v>
+      </c>
+      <c r="J138" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="K138" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="L138" t="n">
+        <v>-135</v>
+      </c>
+      <c r="M138" t="n">
+        <v>21.5</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="n">
+        <v>1010</v>
+      </c>
+      <c r="B139" t="n">
+        <v>458</v>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D139" t="inlineStr">
+        <is>
+          <t>Washington</t>
+        </is>
+      </c>
+      <c r="E139" t="n">
+        <v>6</v>
+      </c>
+      <c r="F139" t="n">
+        <v>7</v>
+      </c>
+      <c r="G139" t="n">
+        <v>3</v>
+      </c>
+      <c r="H139" t="n">
+        <v>6</v>
+      </c>
+      <c r="I139" t="n">
+        <v>22</v>
+      </c>
+      <c r="J139" t="n">
+        <v>43.5</v>
+      </c>
+      <c r="K139" t="n">
+        <v>43</v>
+      </c>
+      <c r="L139" t="n">
+        <v>115</v>
+      </c>
+      <c r="M139" t="n">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="n">
+        <v>1010</v>
+      </c>
+      <c r="B140" t="n">
+        <v>459</v>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D140" t="inlineStr">
+        <is>
+          <t>Tennessee</t>
+        </is>
+      </c>
+      <c r="E140" t="n">
+        <v>7</v>
+      </c>
+      <c r="F140" t="n">
+        <v>17</v>
+      </c>
+      <c r="G140" t="n">
+        <v>7</v>
+      </c>
+      <c r="H140" t="n">
+        <v>6</v>
+      </c>
+      <c r="I140" t="n">
+        <v>37</v>
+      </c>
+      <c r="J140" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="K140" t="n">
+        <v>4</v>
+      </c>
+      <c r="L140" t="n">
+        <v>-200</v>
+      </c>
+      <c r="M140" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="n">
+        <v>1010</v>
+      </c>
+      <c r="B141" t="n">
+        <v>460</v>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D141" t="inlineStr">
+        <is>
+          <t>Jacksonville</t>
+        </is>
+      </c>
+      <c r="E141" t="n">
+        <v>6</v>
+      </c>
+      <c r="F141" t="n">
+        <v>7</v>
+      </c>
+      <c r="G141" t="n">
+        <v>0</v>
+      </c>
+      <c r="H141" t="n">
+        <v>6</v>
+      </c>
+      <c r="I141" t="n">
+        <v>19</v>
+      </c>
+      <c r="J141" t="n">
+        <v>51.5</v>
+      </c>
+      <c r="K141" t="n">
+        <v>48.5</v>
+      </c>
+      <c r="L141" t="n">
+        <v>175</v>
+      </c>
+      <c r="M141" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="n">
+        <v>1010</v>
+      </c>
+      <c r="B142" t="n">
+        <v>461</v>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D142" t="inlineStr">
+        <is>
+          <t>Detroit</t>
+        </is>
+      </c>
+      <c r="E142" t="n">
+        <v>3</v>
+      </c>
+      <c r="F142" t="n">
+        <v>3</v>
+      </c>
+      <c r="G142" t="n">
+        <v>0</v>
+      </c>
+      <c r="H142" t="n">
+        <v>11</v>
+      </c>
+      <c r="I142" t="n">
+        <v>17</v>
+      </c>
+      <c r="J142" t="n">
+        <v>49.5</v>
+      </c>
+      <c r="K142" t="n">
+        <v>49.5</v>
+      </c>
+      <c r="L142" t="n">
+        <v>350</v>
+      </c>
+      <c r="M142" t="n">
+        <v>23.5</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="n">
+        <v>1010</v>
+      </c>
+      <c r="B143" t="n">
+        <v>462</v>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D143" t="inlineStr">
+        <is>
+          <t>Minnesota</t>
+        </is>
+      </c>
+      <c r="E143" t="n">
+        <v>3</v>
+      </c>
+      <c r="F143" t="n">
+        <v>10</v>
+      </c>
+      <c r="G143" t="n">
+        <v>0</v>
+      </c>
+      <c r="H143" t="n">
+        <v>6</v>
+      </c>
+      <c r="I143" t="n">
+        <v>19</v>
+      </c>
+      <c r="J143" t="n">
+        <v>8</v>
+      </c>
+      <c r="K143" t="n">
+        <v>10</v>
+      </c>
+      <c r="L143" t="n">
+        <v>-420</v>
+      </c>
+      <c r="M143" t="n">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="n">
+        <v>1010</v>
+      </c>
+      <c r="B144" t="n">
+        <v>463</v>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D144" t="inlineStr">
+        <is>
+          <t>Denver</t>
+        </is>
+      </c>
+      <c r="E144" t="n">
+        <v>3</v>
+      </c>
+      <c r="F144" t="n">
+        <v>3</v>
+      </c>
+      <c r="G144" t="n">
+        <v>0</v>
+      </c>
+      <c r="H144" t="n">
+        <v>13</v>
+      </c>
+      <c r="I144" t="n">
+        <v>19</v>
+      </c>
+      <c r="J144" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="K144" t="n">
+        <v>1</v>
+      </c>
+      <c r="L144" t="n">
+        <v>-125</v>
+      </c>
+      <c r="M144" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="n">
+        <v>1010</v>
+      </c>
+      <c r="B145" t="n">
+        <v>464</v>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D145" t="inlineStr">
+        <is>
+          <t>Pittsburgh</t>
+        </is>
+      </c>
+      <c r="E145" t="n">
+        <v>7</v>
+      </c>
+      <c r="F145" t="n">
+        <v>10</v>
+      </c>
+      <c r="G145" t="n">
+        <v>7</v>
+      </c>
+      <c r="H145" t="n">
+        <v>3</v>
+      </c>
+      <c r="I145" t="n">
+        <v>27</v>
+      </c>
+      <c r="J145" t="n">
+        <v>42</v>
+      </c>
+      <c r="K145" t="n">
+        <v>40</v>
+      </c>
+      <c r="L145" t="n">
+        <v>105</v>
+      </c>
+      <c r="M145" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="n">
+        <v>1010</v>
+      </c>
+      <c r="B146" t="n">
+        <v>465</v>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D146" t="inlineStr">
+        <is>
+          <t>GreenBay</t>
+        </is>
+      </c>
+      <c r="E146" t="n">
+        <v>0</v>
+      </c>
+      <c r="F146" t="n">
+        <v>16</v>
+      </c>
+      <c r="G146" t="n">
+        <v>3</v>
+      </c>
+      <c r="H146" t="n">
+        <v>3</v>
+      </c>
+      <c r="I146" t="n">
+        <v>25</v>
+      </c>
+      <c r="J146" t="n">
+        <v>3</v>
+      </c>
+      <c r="K146" t="n">
+        <v>1</v>
+      </c>
+      <c r="L146" t="n">
+        <v>-130</v>
+      </c>
+      <c r="M146" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="n">
+        <v>1010</v>
+      </c>
+      <c r="B147" t="n">
+        <v>466</v>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D147" t="inlineStr">
+        <is>
+          <t>Cincinnati</t>
+        </is>
+      </c>
+      <c r="E147" t="n">
+        <v>7</v>
+      </c>
+      <c r="F147" t="n">
+        <v>7</v>
+      </c>
+      <c r="G147" t="n">
+        <v>0</v>
+      </c>
+      <c r="H147" t="n">
+        <v>8</v>
+      </c>
+      <c r="I147" t="n">
+        <v>22</v>
+      </c>
+      <c r="J147" t="n">
+        <v>48.5</v>
+      </c>
+      <c r="K147" t="n">
+        <v>50</v>
+      </c>
+      <c r="L147" t="n">
+        <v>110</v>
+      </c>
+      <c r="M147" t="n">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="n">
+        <v>1010</v>
+      </c>
+      <c r="B148" t="n">
+        <v>467</v>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D148" t="inlineStr">
+        <is>
+          <t>NewEngland</t>
+        </is>
+      </c>
+      <c r="E148" t="n">
+        <v>0</v>
+      </c>
+      <c r="F148" t="n">
+        <v>9</v>
+      </c>
+      <c r="G148" t="n">
+        <v>6</v>
+      </c>
+      <c r="H148" t="n">
+        <v>10</v>
+      </c>
+      <c r="I148" t="n">
+        <v>25</v>
+      </c>
+      <c r="J148" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="K148" t="n">
+        <v>9</v>
+      </c>
+      <c r="L148" t="n">
+        <v>-360</v>
+      </c>
+      <c r="M148" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="n">
+        <v>1010</v>
+      </c>
+      <c r="B149" t="n">
+        <v>468</v>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>Houston</t>
+        </is>
+      </c>
+      <c r="E149" t="n">
+        <v>6</v>
+      </c>
+      <c r="F149" t="n">
+        <v>9</v>
+      </c>
+      <c r="G149" t="n">
+        <v>7</v>
+      </c>
+      <c r="H149" t="n">
+        <v>0</v>
+      </c>
+      <c r="I149" t="n">
+        <v>22</v>
+      </c>
+      <c r="J149" t="n">
+        <v>42</v>
+      </c>
+      <c r="K149" t="n">
+        <v>39</v>
+      </c>
+      <c r="L149" t="n">
+        <v>300</v>
+      </c>
+      <c r="M149" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="n">
+        <v>1010</v>
+      </c>
+      <c r="B150" t="n">
+        <v>469</v>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D150" t="inlineStr">
+        <is>
+          <t>Chicago</t>
+        </is>
+      </c>
+      <c r="E150" t="n">
+        <v>0</v>
+      </c>
+      <c r="F150" t="n">
+        <v>14</v>
+      </c>
+      <c r="G150" t="n">
+        <v>0</v>
+      </c>
+      <c r="H150" t="n">
+        <v>6</v>
+      </c>
+      <c r="I150" t="n">
+        <v>20</v>
+      </c>
+      <c r="J150" t="n">
+        <v>45.5</v>
+      </c>
+      <c r="K150" t="n">
+        <v>46</v>
+      </c>
+      <c r="L150" t="n">
+        <v>200</v>
+      </c>
+      <c r="M150" t="n">
+        <v>23.5</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="n">
+        <v>1010</v>
+      </c>
+      <c r="B151" t="n">
+        <v>470</v>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D151" t="inlineStr">
+        <is>
+          <t>LasVegas</t>
+        </is>
+      </c>
+      <c r="E151" t="n">
+        <v>3</v>
+      </c>
+      <c r="F151" t="n">
+        <v>0</v>
+      </c>
+      <c r="G151" t="n">
+        <v>0</v>
+      </c>
+      <c r="H151" t="n">
+        <v>6</v>
+      </c>
+      <c r="I151" t="n">
+        <v>9</v>
+      </c>
+      <c r="J151" t="n">
+        <v>7</v>
+      </c>
+      <c r="K151" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="L151" t="n">
+        <v>-240</v>
+      </c>
+      <c r="M151" t="n">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="n">
+        <v>1010</v>
+      </c>
+      <c r="B152" t="n">
+        <v>471</v>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D152" t="inlineStr">
+        <is>
+          <t>Cleveland</t>
+        </is>
+      </c>
+      <c r="E152" t="n">
+        <v>3</v>
+      </c>
+      <c r="F152" t="n">
+        <v>17</v>
+      </c>
+      <c r="G152" t="n">
+        <v>7</v>
+      </c>
+      <c r="H152" t="n">
+        <v>15</v>
+      </c>
+      <c r="I152" t="n">
+        <v>42</v>
+      </c>
+      <c r="J152" t="n">
+        <v>1</v>
+      </c>
+      <c r="K152" t="n">
+        <v>47</v>
+      </c>
+      <c r="L152" t="n">
+        <v>115</v>
+      </c>
+      <c r="M152" t="n">
+        <v>26.5</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="n">
+        <v>1010</v>
+      </c>
+      <c r="B153" t="n">
+        <v>472</v>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D153" t="inlineStr">
+        <is>
+          <t>LAChargers</t>
+        </is>
+      </c>
+      <c r="E153" t="n">
+        <v>7</v>
+      </c>
+      <c r="F153" t="n">
+        <v>6</v>
+      </c>
+      <c r="G153" t="n">
+        <v>8</v>
+      </c>
+      <c r="H153" t="n">
+        <v>26</v>
+      </c>
+      <c r="I153" t="n">
+        <v>47</v>
+      </c>
+      <c r="J153" t="n">
+        <v>50</v>
+      </c>
+      <c r="K153" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="L153" t="n">
+        <v>-135</v>
+      </c>
+      <c r="M153" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="n">
+        <v>1010</v>
+      </c>
+      <c r="B154" t="n">
+        <v>473</v>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D154" t="inlineStr">
+        <is>
+          <t>NYGiants</t>
+        </is>
+      </c>
+      <c r="E154" t="n">
+        <v>0</v>
+      </c>
+      <c r="F154" t="n">
+        <v>10</v>
+      </c>
+      <c r="G154" t="n">
+        <v>3</v>
+      </c>
+      <c r="H154" t="n">
+        <v>7</v>
+      </c>
+      <c r="I154" t="n">
+        <v>20</v>
+      </c>
+      <c r="J154" t="n">
+        <v>49</v>
+      </c>
+      <c r="K154" t="n">
+        <v>53.5</v>
+      </c>
+      <c r="L154" t="n">
+        <v>290</v>
+      </c>
+      <c r="M154" t="n">
+        <v>23.5</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="n">
+        <v>1010</v>
+      </c>
+      <c r="B155" t="n">
+        <v>474</v>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D155" t="inlineStr">
+        <is>
+          <t>Dallas</t>
+        </is>
+      </c>
+      <c r="E155" t="n">
+        <v>3</v>
+      </c>
+      <c r="F155" t="n">
+        <v>14</v>
+      </c>
+      <c r="G155" t="n">
+        <v>10</v>
+      </c>
+      <c r="H155" t="n">
+        <v>17</v>
+      </c>
+      <c r="I155" t="n">
+        <v>44</v>
+      </c>
+      <c r="J155" t="n">
+        <v>8</v>
+      </c>
+      <c r="K155" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="L155" t="n">
+        <v>-350</v>
+      </c>
+      <c r="M155" t="n">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="n">
+        <v>1010</v>
+      </c>
+      <c r="B156" t="n">
+        <v>475</v>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D156" t="inlineStr">
+        <is>
+          <t>SanFrancisco</t>
+        </is>
+      </c>
+      <c r="E156" t="n">
+        <v>0</v>
+      </c>
+      <c r="F156" t="n">
+        <v>0</v>
+      </c>
+      <c r="G156" t="n">
+        <v>7</v>
+      </c>
+      <c r="H156" t="n">
+        <v>3</v>
+      </c>
+      <c r="I156" t="n">
+        <v>10</v>
+      </c>
+      <c r="J156" t="n">
+        <v>52</v>
+      </c>
+      <c r="K156" t="n">
+        <v>48.5</v>
+      </c>
+      <c r="L156" t="n">
+        <v>235</v>
+      </c>
+      <c r="M156" t="n">
+        <v>22.5</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="n">
+        <v>1010</v>
+      </c>
+      <c r="B157" t="n">
+        <v>476</v>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D157" t="inlineStr">
+        <is>
+          <t>Arizona</t>
+        </is>
+      </c>
+      <c r="E157" t="n">
+        <v>7</v>
+      </c>
+      <c r="F157" t="n">
+        <v>3</v>
+      </c>
+      <c r="G157" t="n">
+        <v>0</v>
+      </c>
+      <c r="H157" t="n">
+        <v>7</v>
+      </c>
+      <c r="I157" t="n">
+        <v>17</v>
+      </c>
+      <c r="J157" t="n">
+        <v>2</v>
+      </c>
+      <c r="K157" t="n">
+        <v>6</v>
+      </c>
+      <c r="L157" t="n">
+        <v>-275</v>
+      </c>
+      <c r="M157" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="n">
+        <v>1010</v>
+      </c>
+      <c r="B158" t="n">
+        <v>477</v>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D158" t="inlineStr">
+        <is>
+          <t>Buffalo</t>
+        </is>
+      </c>
+      <c r="E158" t="n">
+        <v>7</v>
+      </c>
+      <c r="F158" t="n">
+        <v>17</v>
+      </c>
+      <c r="G158" t="n">
+        <v>7</v>
+      </c>
+      <c r="H158" t="n">
+        <v>7</v>
+      </c>
+      <c r="I158" t="n">
+        <v>38</v>
+      </c>
+      <c r="J158" t="n">
+        <v>56.5</v>
+      </c>
+      <c r="K158" t="n">
+        <v>57</v>
+      </c>
+      <c r="L158" t="n">
+        <v>120</v>
+      </c>
+      <c r="M158" t="n">
+        <v>28.5</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="n">
+        <v>1010</v>
+      </c>
+      <c r="B159" t="n">
+        <v>478</v>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D159" t="inlineStr">
+        <is>
+          <t>KansasCity</t>
+        </is>
+      </c>
+      <c r="E159" t="n">
+        <v>3</v>
+      </c>
+      <c r="F159" t="n">
+        <v>10</v>
+      </c>
+      <c r="G159" t="n">
+        <v>0</v>
+      </c>
+      <c r="H159" t="n">
+        <v>7</v>
+      </c>
+      <c r="I159" t="n">
+        <v>20</v>
+      </c>
+      <c r="J159" t="n">
+        <v>4</v>
+      </c>
+      <c r="K159" t="n">
+        <v>3</v>
+      </c>
+      <c r="L159" t="n">
+        <v>-140</v>
+      </c>
+      <c r="M159" t="n">
+        <v>4.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
moving files, scraping, and working on baseline models
</commit_message>
<xml_diff>
--- a/Data/Odds/NFL/NFL odds 2021-22.xlsx
+++ b/Data/Odds/NFL/NFL odds 2021-22.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M159"/>
+  <dimension ref="A1:M189"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7632,6 +7632,1358 @@
         <v>4.5</v>
       </c>
     </row>
+    <row r="160">
+      <c r="A160" t="n">
+        <v>1011</v>
+      </c>
+      <c r="B160" t="n">
+        <v>479</v>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D160" t="inlineStr">
+        <is>
+          <t>Indianapolis</t>
+        </is>
+      </c>
+      <c r="E160" t="n">
+        <v>7</v>
+      </c>
+      <c r="F160" t="n">
+        <v>3</v>
+      </c>
+      <c r="G160" t="n">
+        <v>12</v>
+      </c>
+      <c r="H160" t="n">
+        <v>3</v>
+      </c>
+      <c r="I160" t="n">
+        <v>25</v>
+      </c>
+      <c r="J160" t="n">
+        <v>49</v>
+      </c>
+      <c r="K160" t="n">
+        <v>46.5</v>
+      </c>
+      <c r="L160" t="n">
+        <v>290</v>
+      </c>
+      <c r="M160" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="n">
+        <v>1011</v>
+      </c>
+      <c r="B161" t="n">
+        <v>480</v>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D161" t="inlineStr">
+        <is>
+          <t>Baltimore</t>
+        </is>
+      </c>
+      <c r="E161" t="n">
+        <v>0</v>
+      </c>
+      <c r="F161" t="n">
+        <v>3</v>
+      </c>
+      <c r="G161" t="n">
+        <v>6</v>
+      </c>
+      <c r="H161" t="n">
+        <v>16</v>
+      </c>
+      <c r="I161" t="n">
+        <v>31</v>
+      </c>
+      <c r="J161" t="n">
+        <v>6</v>
+      </c>
+      <c r="K161" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="L161" t="n">
+        <v>-350</v>
+      </c>
+      <c r="M161" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="n">
+        <v>1014</v>
+      </c>
+      <c r="B162" t="n">
+        <v>109</v>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D162" t="inlineStr">
+        <is>
+          <t>TampaBay</t>
+        </is>
+      </c>
+      <c r="E162" t="n">
+        <v>14</v>
+      </c>
+      <c r="F162" t="n">
+        <v>7</v>
+      </c>
+      <c r="G162" t="n">
+        <v>7</v>
+      </c>
+      <c r="H162" t="n">
+        <v>0</v>
+      </c>
+      <c r="I162" t="n">
+        <v>28</v>
+      </c>
+      <c r="J162" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="K162" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="L162" t="n">
+        <v>-290</v>
+      </c>
+      <c r="M162" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="n">
+        <v>1014</v>
+      </c>
+      <c r="B163" t="n">
+        <v>110</v>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D163" t="inlineStr">
+        <is>
+          <t>Philadelphia</t>
+        </is>
+      </c>
+      <c r="E163" t="n">
+        <v>7</v>
+      </c>
+      <c r="F163" t="n">
+        <v>0</v>
+      </c>
+      <c r="G163" t="n">
+        <v>7</v>
+      </c>
+      <c r="H163" t="n">
+        <v>8</v>
+      </c>
+      <c r="I163" t="n">
+        <v>22</v>
+      </c>
+      <c r="J163" t="n">
+        <v>52.5</v>
+      </c>
+      <c r="K163" t="n">
+        <v>53</v>
+      </c>
+      <c r="L163" t="n">
+        <v>245</v>
+      </c>
+      <c r="M163" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="n">
+        <v>1017</v>
+      </c>
+      <c r="B164" t="n">
+        <v>251</v>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="D164" t="inlineStr">
+        <is>
+          <t>Miami</t>
+        </is>
+      </c>
+      <c r="E164" t="n">
+        <v>7</v>
+      </c>
+      <c r="F164" t="n">
+        <v>6</v>
+      </c>
+      <c r="G164" t="n">
+        <v>0</v>
+      </c>
+      <c r="H164" t="n">
+        <v>7</v>
+      </c>
+      <c r="I164" t="n">
+        <v>20</v>
+      </c>
+      <c r="J164" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="K164" t="inlineStr">
+        <is>
+          <t>pk</t>
+        </is>
+      </c>
+      <c r="L164" t="n">
+        <v>-125</v>
+      </c>
+      <c r="M164" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="n">
+        <v>1017</v>
+      </c>
+      <c r="B165" t="n">
+        <v>252</v>
+      </c>
+      <c r="C165" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="D165" t="inlineStr">
+        <is>
+          <t>Jacksonville</t>
+        </is>
+      </c>
+      <c r="E165" t="n">
+        <v>3</v>
+      </c>
+      <c r="F165" t="n">
+        <v>7</v>
+      </c>
+      <c r="G165" t="n">
+        <v>7</v>
+      </c>
+      <c r="H165" t="n">
+        <v>6</v>
+      </c>
+      <c r="I165" t="n">
+        <v>23</v>
+      </c>
+      <c r="J165" t="n">
+        <v>43.5</v>
+      </c>
+      <c r="K165" t="n">
+        <v>47</v>
+      </c>
+      <c r="L165" t="n">
+        <v>105</v>
+      </c>
+      <c r="M165" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="n">
+        <v>1017</v>
+      </c>
+      <c r="B166" t="n">
+        <v>253</v>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D166" t="inlineStr">
+        <is>
+          <t>Houston</t>
+        </is>
+      </c>
+      <c r="E166" t="n">
+        <v>0</v>
+      </c>
+      <c r="F166" t="n">
+        <v>3</v>
+      </c>
+      <c r="G166" t="n">
+        <v>0</v>
+      </c>
+      <c r="H166" t="n">
+        <v>0</v>
+      </c>
+      <c r="I166" t="n">
+        <v>3</v>
+      </c>
+      <c r="J166" t="n">
+        <v>43.5</v>
+      </c>
+      <c r="K166" t="n">
+        <v>44.5</v>
+      </c>
+      <c r="L166" t="n">
+        <v>450</v>
+      </c>
+      <c r="M166" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="n">
+        <v>1017</v>
+      </c>
+      <c r="B167" t="n">
+        <v>254</v>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D167" t="inlineStr">
+        <is>
+          <t>Indianapolis</t>
+        </is>
+      </c>
+      <c r="E167" t="n">
+        <v>7</v>
+      </c>
+      <c r="F167" t="n">
+        <v>3</v>
+      </c>
+      <c r="G167" t="n">
+        <v>14</v>
+      </c>
+      <c r="H167" t="n">
+        <v>7</v>
+      </c>
+      <c r="I167" t="n">
+        <v>31</v>
+      </c>
+      <c r="J167" t="n">
+        <v>11</v>
+      </c>
+      <c r="K167" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="L167" t="n">
+        <v>-600</v>
+      </c>
+      <c r="M167" t="n">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="n">
+        <v>1017</v>
+      </c>
+      <c r="B168" t="n">
+        <v>255</v>
+      </c>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D168" t="inlineStr">
+        <is>
+          <t>GreenBay</t>
+        </is>
+      </c>
+      <c r="E168" t="n">
+        <v>0</v>
+      </c>
+      <c r="F168" t="n">
+        <v>10</v>
+      </c>
+      <c r="G168" t="n">
+        <v>7</v>
+      </c>
+      <c r="H168" t="n">
+        <v>7</v>
+      </c>
+      <c r="I168" t="n">
+        <v>24</v>
+      </c>
+      <c r="J168" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="K168" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="L168" t="n">
+        <v>-240</v>
+      </c>
+      <c r="M168" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="n">
+        <v>1017</v>
+      </c>
+      <c r="B169" t="n">
+        <v>256</v>
+      </c>
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D169" t="inlineStr">
+        <is>
+          <t>Chicago</t>
+        </is>
+      </c>
+      <c r="E169" t="n">
+        <v>7</v>
+      </c>
+      <c r="F169" t="n">
+        <v>0</v>
+      </c>
+      <c r="G169" t="n">
+        <v>0</v>
+      </c>
+      <c r="H169" t="n">
+        <v>7</v>
+      </c>
+      <c r="I169" t="n">
+        <v>14</v>
+      </c>
+      <c r="J169" t="n">
+        <v>46</v>
+      </c>
+      <c r="K169" t="n">
+        <v>44</v>
+      </c>
+      <c r="L169" t="n">
+        <v>200</v>
+      </c>
+      <c r="M169" t="n">
+        <v>21.5</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="n">
+        <v>1017</v>
+      </c>
+      <c r="B170" t="n">
+        <v>257</v>
+      </c>
+      <c r="C170" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D170" t="inlineStr">
+        <is>
+          <t>KansasCity</t>
+        </is>
+      </c>
+      <c r="E170" t="n">
+        <v>7</v>
+      </c>
+      <c r="F170" t="n">
+        <v>3</v>
+      </c>
+      <c r="G170" t="n">
+        <v>7</v>
+      </c>
+      <c r="H170" t="n">
+        <v>14</v>
+      </c>
+      <c r="I170" t="n">
+        <v>31</v>
+      </c>
+      <c r="J170" t="n">
+        <v>6</v>
+      </c>
+      <c r="K170" t="n">
+        <v>7</v>
+      </c>
+      <c r="L170" t="n">
+        <v>-280</v>
+      </c>
+      <c r="M170" t="n">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="n">
+        <v>1017</v>
+      </c>
+      <c r="B171" t="n">
+        <v>258</v>
+      </c>
+      <c r="C171" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D171" t="inlineStr">
+        <is>
+          <t>Washington</t>
+        </is>
+      </c>
+      <c r="E171" t="n">
+        <v>3</v>
+      </c>
+      <c r="F171" t="n">
+        <v>10</v>
+      </c>
+      <c r="G171" t="n">
+        <v>0</v>
+      </c>
+      <c r="H171" t="n">
+        <v>0</v>
+      </c>
+      <c r="I171" t="n">
+        <v>13</v>
+      </c>
+      <c r="J171" t="n">
+        <v>54</v>
+      </c>
+      <c r="K171" t="n">
+        <v>54</v>
+      </c>
+      <c r="L171" t="n">
+        <v>240</v>
+      </c>
+      <c r="M171" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="n">
+        <v>1017</v>
+      </c>
+      <c r="B172" t="n">
+        <v>259</v>
+      </c>
+      <c r="C172" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D172" t="inlineStr">
+        <is>
+          <t>Minnesota</t>
+        </is>
+      </c>
+      <c r="E172" t="n">
+        <v>6</v>
+      </c>
+      <c r="F172" t="n">
+        <v>6</v>
+      </c>
+      <c r="G172" t="n">
+        <v>13</v>
+      </c>
+      <c r="H172" t="n">
+        <v>3</v>
+      </c>
+      <c r="I172" t="n">
+        <v>34</v>
+      </c>
+      <c r="J172" t="n">
+        <v>47.5</v>
+      </c>
+      <c r="K172" t="n">
+        <v>1</v>
+      </c>
+      <c r="L172" t="n">
+        <v>-135</v>
+      </c>
+      <c r="M172" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="n">
+        <v>1017</v>
+      </c>
+      <c r="B173" t="n">
+        <v>260</v>
+      </c>
+      <c r="C173" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D173" t="inlineStr">
+        <is>
+          <t>Carolina</t>
+        </is>
+      </c>
+      <c r="E173" t="n">
+        <v>7</v>
+      </c>
+      <c r="F173" t="n">
+        <v>3</v>
+      </c>
+      <c r="G173" t="n">
+        <v>7</v>
+      </c>
+      <c r="H173" t="n">
+        <v>11</v>
+      </c>
+      <c r="I173" t="n">
+        <v>28</v>
+      </c>
+      <c r="J173" t="n">
+        <v>1</v>
+      </c>
+      <c r="K173" t="n">
+        <v>45</v>
+      </c>
+      <c r="L173" t="n">
+        <v>115</v>
+      </c>
+      <c r="M173" t="n">
+        <v>21.5</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="n">
+        <v>1017</v>
+      </c>
+      <c r="B174" t="n">
+        <v>261</v>
+      </c>
+      <c r="C174" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D174" t="inlineStr">
+        <is>
+          <t>LAChargers</t>
+        </is>
+      </c>
+      <c r="E174" t="n">
+        <v>0</v>
+      </c>
+      <c r="F174" t="n">
+        <v>6</v>
+      </c>
+      <c r="G174" t="n">
+        <v>0</v>
+      </c>
+      <c r="H174" t="n">
+        <v>0</v>
+      </c>
+      <c r="I174" t="n">
+        <v>6</v>
+      </c>
+      <c r="J174" t="n">
+        <v>48</v>
+      </c>
+      <c r="K174" t="n">
+        <v>51</v>
+      </c>
+      <c r="L174" t="n">
+        <v>135</v>
+      </c>
+      <c r="M174" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="n">
+        <v>1017</v>
+      </c>
+      <c r="B175" t="n">
+        <v>262</v>
+      </c>
+      <c r="C175" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D175" t="inlineStr">
+        <is>
+          <t>Baltimore</t>
+        </is>
+      </c>
+      <c r="E175" t="n">
+        <v>7</v>
+      </c>
+      <c r="F175" t="n">
+        <v>10</v>
+      </c>
+      <c r="G175" t="n">
+        <v>10</v>
+      </c>
+      <c r="H175" t="n">
+        <v>7</v>
+      </c>
+      <c r="I175" t="n">
+        <v>34</v>
+      </c>
+      <c r="J175" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="K175" t="n">
+        <v>3</v>
+      </c>
+      <c r="L175" t="n">
+        <v>-155</v>
+      </c>
+      <c r="M175" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="n">
+        <v>1017</v>
+      </c>
+      <c r="B176" t="n">
+        <v>263</v>
+      </c>
+      <c r="C176" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D176" t="inlineStr">
+        <is>
+          <t>Cincinnati</t>
+        </is>
+      </c>
+      <c r="E176" t="n">
+        <v>7</v>
+      </c>
+      <c r="F176" t="n">
+        <v>3</v>
+      </c>
+      <c r="G176" t="n">
+        <v>10</v>
+      </c>
+      <c r="H176" t="n">
+        <v>14</v>
+      </c>
+      <c r="I176" t="n">
+        <v>34</v>
+      </c>
+      <c r="J176" t="n">
+        <v>3</v>
+      </c>
+      <c r="K176" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="L176" t="n">
+        <v>-185</v>
+      </c>
+      <c r="M176" t="n">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="n">
+        <v>1017</v>
+      </c>
+      <c r="B177" t="n">
+        <v>264</v>
+      </c>
+      <c r="C177" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D177" t="inlineStr">
+        <is>
+          <t>Detroit</t>
+        </is>
+      </c>
+      <c r="E177" t="n">
+        <v>0</v>
+      </c>
+      <c r="F177" t="n">
+        <v>0</v>
+      </c>
+      <c r="G177" t="n">
+        <v>0</v>
+      </c>
+      <c r="H177" t="n">
+        <v>11</v>
+      </c>
+      <c r="I177" t="n">
+        <v>11</v>
+      </c>
+      <c r="J177" t="n">
+        <v>49</v>
+      </c>
+      <c r="K177" t="n">
+        <v>46.5</v>
+      </c>
+      <c r="L177" t="n">
+        <v>165</v>
+      </c>
+      <c r="M177" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="n">
+        <v>1017</v>
+      </c>
+      <c r="B178" t="n">
+        <v>265</v>
+      </c>
+      <c r="C178" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D178" t="inlineStr">
+        <is>
+          <t>LARams</t>
+        </is>
+      </c>
+      <c r="E178" t="n">
+        <v>0</v>
+      </c>
+      <c r="F178" t="n">
+        <v>28</v>
+      </c>
+      <c r="G178" t="n">
+        <v>3</v>
+      </c>
+      <c r="H178" t="n">
+        <v>7</v>
+      </c>
+      <c r="I178" t="n">
+        <v>38</v>
+      </c>
+      <c r="J178" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="K178" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="L178" t="n">
+        <v>-350</v>
+      </c>
+      <c r="M178" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="n">
+        <v>1017</v>
+      </c>
+      <c r="B179" t="n">
+        <v>266</v>
+      </c>
+      <c r="C179" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D179" t="inlineStr">
+        <is>
+          <t>NYGiants</t>
+        </is>
+      </c>
+      <c r="E179" t="n">
+        <v>3</v>
+      </c>
+      <c r="F179" t="n">
+        <v>0</v>
+      </c>
+      <c r="G179" t="n">
+        <v>0</v>
+      </c>
+      <c r="H179" t="n">
+        <v>8</v>
+      </c>
+      <c r="I179" t="n">
+        <v>11</v>
+      </c>
+      <c r="J179" t="n">
+        <v>50</v>
+      </c>
+      <c r="K179" t="n">
+        <v>49.5</v>
+      </c>
+      <c r="L179" t="n">
+        <v>290</v>
+      </c>
+      <c r="M179" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="n">
+        <v>1017</v>
+      </c>
+      <c r="B180" t="n">
+        <v>267</v>
+      </c>
+      <c r="C180" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D180" t="inlineStr">
+        <is>
+          <t>Arizona</t>
+        </is>
+      </c>
+      <c r="E180" t="n">
+        <v>7</v>
+      </c>
+      <c r="F180" t="n">
+        <v>16</v>
+      </c>
+      <c r="G180" t="n">
+        <v>7</v>
+      </c>
+      <c r="H180" t="n">
+        <v>7</v>
+      </c>
+      <c r="I180" t="n">
+        <v>37</v>
+      </c>
+      <c r="J180" t="n">
+        <v>53</v>
+      </c>
+      <c r="K180" t="n">
+        <v>48</v>
+      </c>
+      <c r="L180" t="n">
+        <v>120</v>
+      </c>
+      <c r="M180" t="n">
+        <v>25.5</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="n">
+        <v>1017</v>
+      </c>
+      <c r="B181" t="n">
+        <v>268</v>
+      </c>
+      <c r="C181" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D181" t="inlineStr">
+        <is>
+          <t>Cleveland</t>
+        </is>
+      </c>
+      <c r="E181" t="n">
+        <v>0</v>
+      </c>
+      <c r="F181" t="n">
+        <v>14</v>
+      </c>
+      <c r="G181" t="n">
+        <v>0</v>
+      </c>
+      <c r="H181" t="n">
+        <v>0</v>
+      </c>
+      <c r="I181" t="n">
+        <v>14</v>
+      </c>
+      <c r="J181" t="n">
+        <v>3</v>
+      </c>
+      <c r="K181" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="L181" t="n">
+        <v>-140</v>
+      </c>
+      <c r="M181" t="n">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="n">
+        <v>1017</v>
+      </c>
+      <c r="B182" t="n">
+        <v>269</v>
+      </c>
+      <c r="C182" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D182" t="inlineStr">
+        <is>
+          <t>LasVegas</t>
+        </is>
+      </c>
+      <c r="E182" t="n">
+        <v>10</v>
+      </c>
+      <c r="F182" t="n">
+        <v>7</v>
+      </c>
+      <c r="G182" t="n">
+        <v>14</v>
+      </c>
+      <c r="H182" t="n">
+        <v>3</v>
+      </c>
+      <c r="I182" t="n">
+        <v>34</v>
+      </c>
+      <c r="J182" t="n">
+        <v>44</v>
+      </c>
+      <c r="K182" t="n">
+        <v>45</v>
+      </c>
+      <c r="L182" t="n">
+        <v>180</v>
+      </c>
+      <c r="M182" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="n">
+        <v>1017</v>
+      </c>
+      <c r="B183" t="n">
+        <v>270</v>
+      </c>
+      <c r="C183" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D183" t="inlineStr">
+        <is>
+          <t>Denver</t>
+        </is>
+      </c>
+      <c r="E183" t="n">
+        <v>7</v>
+      </c>
+      <c r="F183" t="n">
+        <v>0</v>
+      </c>
+      <c r="G183" t="n">
+        <v>3</v>
+      </c>
+      <c r="H183" t="n">
+        <v>14</v>
+      </c>
+      <c r="I183" t="n">
+        <v>24</v>
+      </c>
+      <c r="J183" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="K183" t="n">
+        <v>5</v>
+      </c>
+      <c r="L183" t="n">
+        <v>-210</v>
+      </c>
+      <c r="M183" t="n">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="n">
+        <v>1017</v>
+      </c>
+      <c r="B184" t="n">
+        <v>271</v>
+      </c>
+      <c r="C184" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D184" t="inlineStr">
+        <is>
+          <t>Dallas</t>
+        </is>
+      </c>
+      <c r="E184" t="n">
+        <v>7</v>
+      </c>
+      <c r="F184" t="n">
+        <v>3</v>
+      </c>
+      <c r="G184" t="n">
+        <v>7</v>
+      </c>
+      <c r="H184" t="n">
+        <v>12</v>
+      </c>
+      <c r="I184" t="n">
+        <v>35</v>
+      </c>
+      <c r="J184" t="n">
+        <v>1</v>
+      </c>
+      <c r="K184" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="L184" t="n">
+        <v>-190</v>
+      </c>
+      <c r="M184" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="n">
+        <v>1017</v>
+      </c>
+      <c r="B185" t="n">
+        <v>272</v>
+      </c>
+      <c r="C185" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D185" t="inlineStr">
+        <is>
+          <t>NewEngland</t>
+        </is>
+      </c>
+      <c r="E185" t="n">
+        <v>14</v>
+      </c>
+      <c r="F185" t="n">
+        <v>0</v>
+      </c>
+      <c r="G185" t="n">
+        <v>0</v>
+      </c>
+      <c r="H185" t="n">
+        <v>15</v>
+      </c>
+      <c r="I185" t="n">
+        <v>29</v>
+      </c>
+      <c r="J185" t="n">
+        <v>48</v>
+      </c>
+      <c r="K185" t="n">
+        <v>50.5</v>
+      </c>
+      <c r="L185" t="n">
+        <v>170</v>
+      </c>
+      <c r="M185" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="n">
+        <v>1017</v>
+      </c>
+      <c r="B186" t="n">
+        <v>273</v>
+      </c>
+      <c r="C186" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D186" t="inlineStr">
+        <is>
+          <t>Seattle</t>
+        </is>
+      </c>
+      <c r="E186" t="n">
+        <v>0</v>
+      </c>
+      <c r="F186" t="n">
+        <v>0</v>
+      </c>
+      <c r="G186" t="n">
+        <v>14</v>
+      </c>
+      <c r="H186" t="n">
+        <v>6</v>
+      </c>
+      <c r="I186" t="n">
+        <v>20</v>
+      </c>
+      <c r="J186" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="K186" t="n">
+        <v>43</v>
+      </c>
+      <c r="L186" t="n">
+        <v>200</v>
+      </c>
+      <c r="M186" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="n">
+        <v>1017</v>
+      </c>
+      <c r="B187" t="n">
+        <v>274</v>
+      </c>
+      <c r="C187" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D187" t="inlineStr">
+        <is>
+          <t>Pittsburgh</t>
+        </is>
+      </c>
+      <c r="E187" t="n">
+        <v>0</v>
+      </c>
+      <c r="F187" t="n">
+        <v>14</v>
+      </c>
+      <c r="G187" t="n">
+        <v>3</v>
+      </c>
+      <c r="H187" t="n">
+        <v>3</v>
+      </c>
+      <c r="I187" t="n">
+        <v>23</v>
+      </c>
+      <c r="J187" t="n">
+        <v>48</v>
+      </c>
+      <c r="K187" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="L187" t="n">
+        <v>-240</v>
+      </c>
+      <c r="M187" t="n">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="n">
+        <v>1018</v>
+      </c>
+      <c r="B188" t="n">
+        <v>275</v>
+      </c>
+      <c r="C188" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D188" t="inlineStr">
+        <is>
+          <t>Buffalo</t>
+        </is>
+      </c>
+      <c r="E188" t="n">
+        <v>3</v>
+      </c>
+      <c r="F188" t="n">
+        <v>17</v>
+      </c>
+      <c r="G188" t="n">
+        <v>11</v>
+      </c>
+      <c r="H188" t="n">
+        <v>0</v>
+      </c>
+      <c r="I188" t="n">
+        <v>31</v>
+      </c>
+      <c r="J188" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="K188" t="n">
+        <v>7</v>
+      </c>
+      <c r="L188" t="n">
+        <v>-265</v>
+      </c>
+      <c r="M188" t="n">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="n">
+        <v>1018</v>
+      </c>
+      <c r="B189" t="n">
+        <v>276</v>
+      </c>
+      <c r="C189" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D189" t="inlineStr">
+        <is>
+          <t>Tennessee</t>
+        </is>
+      </c>
+      <c r="E189" t="n">
+        <v>0</v>
+      </c>
+      <c r="F189" t="n">
+        <v>17</v>
+      </c>
+      <c r="G189" t="n">
+        <v>7</v>
+      </c>
+      <c r="H189" t="n">
+        <v>10</v>
+      </c>
+      <c r="I189" t="n">
+        <v>34</v>
+      </c>
+      <c r="J189" t="n">
+        <v>53</v>
+      </c>
+      <c r="K189" t="n">
+        <v>53.5</v>
+      </c>
+      <c r="L189" t="n">
+        <v>225</v>
+      </c>
+      <c r="M189" t="n">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
scraping and building baselines
</commit_message>
<xml_diff>
--- a/Data/Odds/NFL/NFL odds 2021-22.xlsx
+++ b/Data/Odds/NFL/NFL odds 2021-22.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M189"/>
+  <dimension ref="A1:M215"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8984,6 +8984,1182 @@
         <v>26</v>
       </c>
     </row>
+    <row r="190">
+      <c r="A190" t="n">
+        <v>1021</v>
+      </c>
+      <c r="B190" t="n">
+        <v>309</v>
+      </c>
+      <c r="C190" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D190" t="inlineStr">
+        <is>
+          <t>Denver</t>
+        </is>
+      </c>
+      <c r="E190" t="n">
+        <v>0</v>
+      </c>
+      <c r="F190" t="n">
+        <v>0</v>
+      </c>
+      <c r="G190" t="n">
+        <v>7</v>
+      </c>
+      <c r="H190" t="n">
+        <v>7</v>
+      </c>
+      <c r="I190" t="n">
+        <v>14</v>
+      </c>
+      <c r="J190" t="n">
+        <v>44.5</v>
+      </c>
+      <c r="K190" t="n">
+        <v>40</v>
+      </c>
+      <c r="L190" t="n">
+        <v>110</v>
+      </c>
+      <c r="M190" t="n">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="n">
+        <v>1021</v>
+      </c>
+      <c r="B191" t="n">
+        <v>310</v>
+      </c>
+      <c r="C191" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D191" t="inlineStr">
+        <is>
+          <t>Cleveland</t>
+        </is>
+      </c>
+      <c r="E191" t="n">
+        <v>10</v>
+      </c>
+      <c r="F191" t="n">
+        <v>0</v>
+      </c>
+      <c r="G191" t="n">
+        <v>7</v>
+      </c>
+      <c r="H191" t="n">
+        <v>0</v>
+      </c>
+      <c r="I191" t="n">
+        <v>17</v>
+      </c>
+      <c r="J191" t="n">
+        <v>6</v>
+      </c>
+      <c r="K191" t="inlineStr">
+        <is>
+          <t>pk</t>
+        </is>
+      </c>
+      <c r="L191" t="n">
+        <v>-130</v>
+      </c>
+      <c r="M191" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="n">
+        <v>1024</v>
+      </c>
+      <c r="B192" t="n">
+        <v>451</v>
+      </c>
+      <c r="C192" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D192" t="inlineStr">
+        <is>
+          <t>Cincinnati</t>
+        </is>
+      </c>
+      <c r="E192" t="n">
+        <v>3</v>
+      </c>
+      <c r="F192" t="n">
+        <v>10</v>
+      </c>
+      <c r="G192" t="n">
+        <v>14</v>
+      </c>
+      <c r="H192" t="n">
+        <v>14</v>
+      </c>
+      <c r="I192" t="n">
+        <v>41</v>
+      </c>
+      <c r="J192" t="n">
+        <v>48</v>
+      </c>
+      <c r="K192" t="n">
+        <v>46</v>
+      </c>
+      <c r="L192" t="n">
+        <v>230</v>
+      </c>
+      <c r="M192" t="n">
+        <v>23.5</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="n">
+        <v>1024</v>
+      </c>
+      <c r="B193" t="n">
+        <v>452</v>
+      </c>
+      <c r="C193" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D193" t="inlineStr">
+        <is>
+          <t>Baltimore</t>
+        </is>
+      </c>
+      <c r="E193" t="n">
+        <v>0</v>
+      </c>
+      <c r="F193" t="n">
+        <v>10</v>
+      </c>
+      <c r="G193" t="n">
+        <v>7</v>
+      </c>
+      <c r="H193" t="n">
+        <v>0</v>
+      </c>
+      <c r="I193" t="n">
+        <v>17</v>
+      </c>
+      <c r="J193" t="n">
+        <v>7</v>
+      </c>
+      <c r="K193" t="n">
+        <v>7</v>
+      </c>
+      <c r="L193" t="n">
+        <v>-270</v>
+      </c>
+      <c r="M193" t="n">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="n">
+        <v>1024</v>
+      </c>
+      <c r="B194" t="n">
+        <v>453</v>
+      </c>
+      <c r="C194" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D194" t="inlineStr">
+        <is>
+          <t>Carolina</t>
+        </is>
+      </c>
+      <c r="E194" t="n">
+        <v>3</v>
+      </c>
+      <c r="F194" t="n">
+        <v>0</v>
+      </c>
+      <c r="G194" t="n">
+        <v>0</v>
+      </c>
+      <c r="H194" t="n">
+        <v>0</v>
+      </c>
+      <c r="I194" t="n">
+        <v>3</v>
+      </c>
+      <c r="J194" t="n">
+        <v>3</v>
+      </c>
+      <c r="K194" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="L194" t="n">
+        <v>-150</v>
+      </c>
+      <c r="M194" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="n">
+        <v>1024</v>
+      </c>
+      <c r="B195" t="n">
+        <v>454</v>
+      </c>
+      <c r="C195" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D195" t="inlineStr">
+        <is>
+          <t>NYGiants</t>
+        </is>
+      </c>
+      <c r="E195" t="n">
+        <v>0</v>
+      </c>
+      <c r="F195" t="n">
+        <v>5</v>
+      </c>
+      <c r="G195" t="n">
+        <v>7</v>
+      </c>
+      <c r="H195" t="n">
+        <v>13</v>
+      </c>
+      <c r="I195" t="n">
+        <v>25</v>
+      </c>
+      <c r="J195" t="n">
+        <v>45.5</v>
+      </c>
+      <c r="K195" t="n">
+        <v>42.5</v>
+      </c>
+      <c r="L195" t="n">
+        <v>130</v>
+      </c>
+      <c r="M195" t="n">
+        <v>20.5</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="n">
+        <v>1024</v>
+      </c>
+      <c r="B196" t="n">
+        <v>455</v>
+      </c>
+      <c r="C196" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D196" t="inlineStr">
+        <is>
+          <t>Washington</t>
+        </is>
+      </c>
+      <c r="E196" t="n">
+        <v>7</v>
+      </c>
+      <c r="F196" t="n">
+        <v>0</v>
+      </c>
+      <c r="G196" t="n">
+        <v>0</v>
+      </c>
+      <c r="H196" t="n">
+        <v>3</v>
+      </c>
+      <c r="I196" t="n">
+        <v>10</v>
+      </c>
+      <c r="J196" t="n">
+        <v>50</v>
+      </c>
+      <c r="K196" t="n">
+        <v>48</v>
+      </c>
+      <c r="L196" t="n">
+        <v>350</v>
+      </c>
+      <c r="M196" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="n">
+        <v>1024</v>
+      </c>
+      <c r="B197" t="n">
+        <v>456</v>
+      </c>
+      <c r="C197" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D197" t="inlineStr">
+        <is>
+          <t>GreenBay</t>
+        </is>
+      </c>
+      <c r="E197" t="n">
+        <v>7</v>
+      </c>
+      <c r="F197" t="n">
+        <v>7</v>
+      </c>
+      <c r="G197" t="n">
+        <v>7</v>
+      </c>
+      <c r="H197" t="n">
+        <v>3</v>
+      </c>
+      <c r="I197" t="n">
+        <v>24</v>
+      </c>
+      <c r="J197" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="K197" t="n">
+        <v>10</v>
+      </c>
+      <c r="L197" t="n">
+        <v>-420</v>
+      </c>
+      <c r="M197" t="n">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="n">
+        <v>1024</v>
+      </c>
+      <c r="B198" t="n">
+        <v>457</v>
+      </c>
+      <c r="C198" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D198" t="inlineStr">
+        <is>
+          <t>KansasCity</t>
+        </is>
+      </c>
+      <c r="E198" t="n">
+        <v>0</v>
+      </c>
+      <c r="F198" t="n">
+        <v>0</v>
+      </c>
+      <c r="G198" t="n">
+        <v>3</v>
+      </c>
+      <c r="H198" t="n">
+        <v>0</v>
+      </c>
+      <c r="I198" t="n">
+        <v>3</v>
+      </c>
+      <c r="J198" t="n">
+        <v>3</v>
+      </c>
+      <c r="K198" t="n">
+        <v>4</v>
+      </c>
+      <c r="L198" t="n">
+        <v>-200</v>
+      </c>
+      <c r="M198" t="n">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="n">
+        <v>1024</v>
+      </c>
+      <c r="B199" t="n">
+        <v>458</v>
+      </c>
+      <c r="C199" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D199" t="inlineStr">
+        <is>
+          <t>Tennessee</t>
+        </is>
+      </c>
+      <c r="E199" t="n">
+        <v>14</v>
+      </c>
+      <c r="F199" t="n">
+        <v>13</v>
+      </c>
+      <c r="G199" t="n">
+        <v>0</v>
+      </c>
+      <c r="H199" t="n">
+        <v>0</v>
+      </c>
+      <c r="I199" t="n">
+        <v>27</v>
+      </c>
+      <c r="J199" t="n">
+        <v>56</v>
+      </c>
+      <c r="K199" t="n">
+        <v>59</v>
+      </c>
+      <c r="L199" t="n">
+        <v>175</v>
+      </c>
+      <c r="M199" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="n">
+        <v>1024</v>
+      </c>
+      <c r="B200" t="n">
+        <v>459</v>
+      </c>
+      <c r="C200" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D200" t="inlineStr">
+        <is>
+          <t>Atlanta</t>
+        </is>
+      </c>
+      <c r="E200" t="n">
+        <v>0</v>
+      </c>
+      <c r="F200" t="n">
+        <v>13</v>
+      </c>
+      <c r="G200" t="n">
+        <v>7</v>
+      </c>
+      <c r="H200" t="n">
+        <v>10</v>
+      </c>
+      <c r="I200" t="n">
+        <v>30</v>
+      </c>
+      <c r="J200" t="n">
+        <v>48</v>
+      </c>
+      <c r="K200" t="inlineStr">
+        <is>
+          <t>pk</t>
+        </is>
+      </c>
+      <c r="L200" t="n">
+        <v>-125</v>
+      </c>
+      <c r="M200" t="n">
+        <v>23.5</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="n">
+        <v>1024</v>
+      </c>
+      <c r="B201" t="n">
+        <v>460</v>
+      </c>
+      <c r="C201" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D201" t="inlineStr">
+        <is>
+          <t>Miami</t>
+        </is>
+      </c>
+      <c r="E201" t="n">
+        <v>7</v>
+      </c>
+      <c r="F201" t="n">
+        <v>0</v>
+      </c>
+      <c r="G201" t="n">
+        <v>7</v>
+      </c>
+      <c r="H201" t="n">
+        <v>14</v>
+      </c>
+      <c r="I201" t="n">
+        <v>28</v>
+      </c>
+      <c r="J201" t="n">
+        <v>3</v>
+      </c>
+      <c r="K201" t="n">
+        <v>47.5</v>
+      </c>
+      <c r="L201" t="n">
+        <v>105</v>
+      </c>
+      <c r="M201" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="n">
+        <v>1024</v>
+      </c>
+      <c r="B202" t="n">
+        <v>461</v>
+      </c>
+      <c r="C202" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D202" t="inlineStr">
+        <is>
+          <t>NYJets</t>
+        </is>
+      </c>
+      <c r="E202" t="n">
+        <v>0</v>
+      </c>
+      <c r="F202" t="n">
+        <v>7</v>
+      </c>
+      <c r="G202" t="n">
+        <v>6</v>
+      </c>
+      <c r="H202" t="n">
+        <v>0</v>
+      </c>
+      <c r="I202" t="n">
+        <v>13</v>
+      </c>
+      <c r="J202" t="n">
+        <v>43.5</v>
+      </c>
+      <c r="K202" t="n">
+        <v>42.5</v>
+      </c>
+      <c r="L202" t="n">
+        <v>280</v>
+      </c>
+      <c r="M202" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="n">
+        <v>1024</v>
+      </c>
+      <c r="B203" t="n">
+        <v>462</v>
+      </c>
+      <c r="C203" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D203" t="inlineStr">
+        <is>
+          <t>NewEngland</t>
+        </is>
+      </c>
+      <c r="E203" t="n">
+        <v>14</v>
+      </c>
+      <c r="F203" t="n">
+        <v>17</v>
+      </c>
+      <c r="G203" t="n">
+        <v>3</v>
+      </c>
+      <c r="H203" t="n">
+        <v>20</v>
+      </c>
+      <c r="I203" t="n">
+        <v>54</v>
+      </c>
+      <c r="J203" t="n">
+        <v>7</v>
+      </c>
+      <c r="K203" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="L203" t="n">
+        <v>-340</v>
+      </c>
+      <c r="M203" t="n">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="n">
+        <v>1024</v>
+      </c>
+      <c r="B204" t="n">
+        <v>463</v>
+      </c>
+      <c r="C204" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D204" t="inlineStr">
+        <is>
+          <t>Detroit</t>
+        </is>
+      </c>
+      <c r="E204" t="n">
+        <v>10</v>
+      </c>
+      <c r="F204" t="n">
+        <v>6</v>
+      </c>
+      <c r="G204" t="n">
+        <v>3</v>
+      </c>
+      <c r="H204" t="n">
+        <v>0</v>
+      </c>
+      <c r="I204" t="n">
+        <v>19</v>
+      </c>
+      <c r="J204" t="n">
+        <v>49.5</v>
+      </c>
+      <c r="K204" t="n">
+        <v>50.5</v>
+      </c>
+      <c r="L204" t="n">
+        <v>900</v>
+      </c>
+      <c r="M204" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="n">
+        <v>1024</v>
+      </c>
+      <c r="B205" t="n">
+        <v>464</v>
+      </c>
+      <c r="C205" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D205" t="inlineStr">
+        <is>
+          <t>LARams</t>
+        </is>
+      </c>
+      <c r="E205" t="n">
+        <v>3</v>
+      </c>
+      <c r="F205" t="n">
+        <v>14</v>
+      </c>
+      <c r="G205" t="n">
+        <v>0</v>
+      </c>
+      <c r="H205" t="n">
+        <v>11</v>
+      </c>
+      <c r="I205" t="n">
+        <v>28</v>
+      </c>
+      <c r="J205" t="n">
+        <v>13.5</v>
+      </c>
+      <c r="K205" t="n">
+        <v>16.5</v>
+      </c>
+      <c r="L205" t="n">
+        <v>-1600</v>
+      </c>
+      <c r="M205" t="n">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="n">
+        <v>1024</v>
+      </c>
+      <c r="B206" t="n">
+        <v>465</v>
+      </c>
+      <c r="C206" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D206" t="inlineStr">
+        <is>
+          <t>Philadelphia</t>
+        </is>
+      </c>
+      <c r="E206" t="n">
+        <v>7</v>
+      </c>
+      <c r="F206" t="n">
+        <v>0</v>
+      </c>
+      <c r="G206" t="n">
+        <v>0</v>
+      </c>
+      <c r="H206" t="n">
+        <v>15</v>
+      </c>
+      <c r="I206" t="n">
+        <v>22</v>
+      </c>
+      <c r="J206" t="n">
+        <v>48.5</v>
+      </c>
+      <c r="K206" t="n">
+        <v>48.5</v>
+      </c>
+      <c r="L206" t="n">
+        <v>-110</v>
+      </c>
+      <c r="M206" t="n">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="n">
+        <v>1024</v>
+      </c>
+      <c r="B207" t="n">
+        <v>466</v>
+      </c>
+      <c r="C207" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D207" t="inlineStr">
+        <is>
+          <t>LasVegas</t>
+        </is>
+      </c>
+      <c r="E207" t="n">
+        <v>0</v>
+      </c>
+      <c r="F207" t="n">
+        <v>17</v>
+      </c>
+      <c r="G207" t="n">
+        <v>13</v>
+      </c>
+      <c r="H207" t="n">
+        <v>3</v>
+      </c>
+      <c r="I207" t="n">
+        <v>33</v>
+      </c>
+      <c r="J207" t="n">
+        <v>3</v>
+      </c>
+      <c r="K207" t="inlineStr">
+        <is>
+          <t>pk</t>
+        </is>
+      </c>
+      <c r="L207" t="n">
+        <v>-110</v>
+      </c>
+      <c r="M207" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="n">
+        <v>1024</v>
+      </c>
+      <c r="B208" t="n">
+        <v>467</v>
+      </c>
+      <c r="C208" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D208" t="inlineStr">
+        <is>
+          <t>Chicago</t>
+        </is>
+      </c>
+      <c r="E208" t="n">
+        <v>0</v>
+      </c>
+      <c r="F208" t="n">
+        <v>3</v>
+      </c>
+      <c r="G208" t="n">
+        <v>0</v>
+      </c>
+      <c r="H208" t="n">
+        <v>0</v>
+      </c>
+      <c r="I208" t="n">
+        <v>3</v>
+      </c>
+      <c r="J208" t="n">
+        <v>49</v>
+      </c>
+      <c r="K208" t="n">
+        <v>47</v>
+      </c>
+      <c r="L208" t="n">
+        <v>500</v>
+      </c>
+      <c r="M208" t="n">
+        <v>20.5</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="n">
+        <v>1024</v>
+      </c>
+      <c r="B209" t="n">
+        <v>468</v>
+      </c>
+      <c r="C209" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D209" t="inlineStr">
+        <is>
+          <t>TampaBay</t>
+        </is>
+      </c>
+      <c r="E209" t="n">
+        <v>21</v>
+      </c>
+      <c r="F209" t="n">
+        <v>14</v>
+      </c>
+      <c r="G209" t="n">
+        <v>0</v>
+      </c>
+      <c r="H209" t="n">
+        <v>3</v>
+      </c>
+      <c r="I209" t="n">
+        <v>38</v>
+      </c>
+      <c r="J209" t="n">
+        <v>10</v>
+      </c>
+      <c r="K209" t="n">
+        <v>13.5</v>
+      </c>
+      <c r="L209" t="n">
+        <v>-700</v>
+      </c>
+      <c r="M209" t="n">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="n">
+        <v>1024</v>
+      </c>
+      <c r="B210" t="n">
+        <v>469</v>
+      </c>
+      <c r="C210" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D210" t="inlineStr">
+        <is>
+          <t>Houston</t>
+        </is>
+      </c>
+      <c r="E210" t="n">
+        <v>2</v>
+      </c>
+      <c r="F210" t="n">
+        <v>3</v>
+      </c>
+      <c r="G210" t="n">
+        <v>0</v>
+      </c>
+      <c r="H210" t="n">
+        <v>0</v>
+      </c>
+      <c r="I210" t="n">
+        <v>5</v>
+      </c>
+      <c r="J210" t="n">
+        <v>49.5</v>
+      </c>
+      <c r="K210" t="n">
+        <v>47.5</v>
+      </c>
+      <c r="L210" t="n">
+        <v>1200</v>
+      </c>
+      <c r="M210" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="n">
+        <v>1024</v>
+      </c>
+      <c r="B211" t="n">
+        <v>470</v>
+      </c>
+      <c r="C211" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D211" t="inlineStr">
+        <is>
+          <t>Arizona</t>
+        </is>
+      </c>
+      <c r="E211" t="n">
+        <v>0</v>
+      </c>
+      <c r="F211" t="n">
+        <v>17</v>
+      </c>
+      <c r="G211" t="n">
+        <v>7</v>
+      </c>
+      <c r="H211" t="n">
+        <v>7</v>
+      </c>
+      <c r="I211" t="n">
+        <v>31</v>
+      </c>
+      <c r="J211" t="n">
+        <v>14.5</v>
+      </c>
+      <c r="K211" t="n">
+        <v>20</v>
+      </c>
+      <c r="L211" t="n">
+        <v>-3000</v>
+      </c>
+      <c r="M211" t="n">
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="n">
+        <v>1024</v>
+      </c>
+      <c r="B212" t="n">
+        <v>471</v>
+      </c>
+      <c r="C212" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D212" t="inlineStr">
+        <is>
+          <t>Indianapolis</t>
+        </is>
+      </c>
+      <c r="E212" t="n">
+        <v>7</v>
+      </c>
+      <c r="F212" t="n">
+        <v>6</v>
+      </c>
+      <c r="G212" t="n">
+        <v>7</v>
+      </c>
+      <c r="H212" t="n">
+        <v>10</v>
+      </c>
+      <c r="I212" t="n">
+        <v>30</v>
+      </c>
+      <c r="J212" t="n">
+        <v>44.5</v>
+      </c>
+      <c r="K212" t="n">
+        <v>41.5</v>
+      </c>
+      <c r="L212" t="n">
+        <v>150</v>
+      </c>
+      <c r="M212" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="n">
+        <v>1024</v>
+      </c>
+      <c r="B213" t="n">
+        <v>472</v>
+      </c>
+      <c r="C213" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D213" t="inlineStr">
+        <is>
+          <t>SanFrancisco</t>
+        </is>
+      </c>
+      <c r="E213" t="n">
+        <v>12</v>
+      </c>
+      <c r="F213" t="n">
+        <v>0</v>
+      </c>
+      <c r="G213" t="n">
+        <v>0</v>
+      </c>
+      <c r="H213" t="n">
+        <v>6</v>
+      </c>
+      <c r="I213" t="n">
+        <v>18</v>
+      </c>
+      <c r="J213" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="K213" t="n">
+        <v>3</v>
+      </c>
+      <c r="L213" t="n">
+        <v>-170</v>
+      </c>
+      <c r="M213" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="n">
+        <v>1025</v>
+      </c>
+      <c r="B214" t="n">
+        <v>473</v>
+      </c>
+      <c r="C214" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D214" t="inlineStr">
+        <is>
+          <t>NewOrleans</t>
+        </is>
+      </c>
+      <c r="E214" t="n">
+        <v>0</v>
+      </c>
+      <c r="F214" t="n">
+        <v>10</v>
+      </c>
+      <c r="G214" t="n">
+        <v>0</v>
+      </c>
+      <c r="H214" t="n">
+        <v>3</v>
+      </c>
+      <c r="I214" t="n">
+        <v>13</v>
+      </c>
+      <c r="J214" t="n">
+        <v>3</v>
+      </c>
+      <c r="K214" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="L214" t="n">
+        <v>-250</v>
+      </c>
+      <c r="M214" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="n">
+        <v>1025</v>
+      </c>
+      <c r="B215" t="n">
+        <v>474</v>
+      </c>
+      <c r="C215" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D215" t="inlineStr">
+        <is>
+          <t>Seattle</t>
+        </is>
+      </c>
+      <c r="E215" t="n">
+        <v>7</v>
+      </c>
+      <c r="F215" t="n">
+        <v>0</v>
+      </c>
+      <c r="G215" t="n">
+        <v>3</v>
+      </c>
+      <c r="H215" t="n">
+        <v>0</v>
+      </c>
+      <c r="I215" t="n">
+        <v>10</v>
+      </c>
+      <c r="J215" t="n">
+        <v>44</v>
+      </c>
+      <c r="K215" t="n">
+        <v>42</v>
+      </c>
+      <c r="L215" t="n">
+        <v>210</v>
+      </c>
+      <c r="M215" t="n">
+        <v>20.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
scraping, running modeling data and saving to data folder now
</commit_message>
<xml_diff>
--- a/Data/Odds/NFL/NFL odds 2021-22.xlsx
+++ b/Data/Odds/NFL/NFL odds 2021-22.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M271"/>
+  <dimension ref="A1:M301"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12686,6 +12686,1358 @@
         <v>8.5</v>
       </c>
     </row>
+    <row r="272">
+      <c r="A272" t="n">
+        <v>1108</v>
+      </c>
+      <c r="B272" t="n">
+        <v>475</v>
+      </c>
+      <c r="C272" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D272" t="inlineStr">
+        <is>
+          <t>Chicago</t>
+        </is>
+      </c>
+      <c r="E272" t="n">
+        <v>0</v>
+      </c>
+      <c r="F272" t="n">
+        <v>3</v>
+      </c>
+      <c r="G272" t="n">
+        <v>3</v>
+      </c>
+      <c r="H272" t="n">
+        <v>21</v>
+      </c>
+      <c r="I272" t="n">
+        <v>27</v>
+      </c>
+      <c r="J272" t="n">
+        <v>40.5</v>
+      </c>
+      <c r="K272" t="n">
+        <v>40</v>
+      </c>
+      <c r="L272" t="n">
+        <v>260</v>
+      </c>
+      <c r="M272" t="n">
+        <v>18.5</v>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" t="n">
+        <v>1108</v>
+      </c>
+      <c r="B273" t="n">
+        <v>476</v>
+      </c>
+      <c r="C273" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D273" t="inlineStr">
+        <is>
+          <t>Pittsburgh</t>
+        </is>
+      </c>
+      <c r="E273" t="n">
+        <v>7</v>
+      </c>
+      <c r="F273" t="n">
+        <v>7</v>
+      </c>
+      <c r="G273" t="n">
+        <v>6</v>
+      </c>
+      <c r="H273" t="n">
+        <v>9</v>
+      </c>
+      <c r="I273" t="n">
+        <v>29</v>
+      </c>
+      <c r="J273" t="n">
+        <v>-5</v>
+      </c>
+      <c r="K273" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="L273" t="n">
+        <v>-310</v>
+      </c>
+      <c r="M273" t="n">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" t="n">
+        <v>1111</v>
+      </c>
+      <c r="B274" t="n">
+        <v>113</v>
+      </c>
+      <c r="C274" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D274" t="inlineStr">
+        <is>
+          <t>Baltimore</t>
+        </is>
+      </c>
+      <c r="E274" t="n">
+        <v>3</v>
+      </c>
+      <c r="F274" t="n">
+        <v>0</v>
+      </c>
+      <c r="G274" t="n">
+        <v>0</v>
+      </c>
+      <c r="H274" t="n">
+        <v>7</v>
+      </c>
+      <c r="I274" t="n">
+        <v>10</v>
+      </c>
+      <c r="J274" t="n">
+        <v>7</v>
+      </c>
+      <c r="K274" t="n">
+        <v>10</v>
+      </c>
+      <c r="L274" t="n">
+        <v>-410</v>
+      </c>
+      <c r="M274" t="n">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="n">
+        <v>1111</v>
+      </c>
+      <c r="B275" t="n">
+        <v>114</v>
+      </c>
+      <c r="C275" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D275" t="inlineStr">
+        <is>
+          <t>Miami</t>
+        </is>
+      </c>
+      <c r="E275" t="n">
+        <v>0</v>
+      </c>
+      <c r="F275" t="n">
+        <v>6</v>
+      </c>
+      <c r="G275" t="n">
+        <v>0</v>
+      </c>
+      <c r="H275" t="n">
+        <v>16</v>
+      </c>
+      <c r="I275" t="n">
+        <v>22</v>
+      </c>
+      <c r="J275" t="n">
+        <v>48</v>
+      </c>
+      <c r="K275" t="n">
+        <v>47</v>
+      </c>
+      <c r="L275" t="n">
+        <v>340</v>
+      </c>
+      <c r="M275" t="n">
+        <v>22.5</v>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="n">
+        <v>1114</v>
+      </c>
+      <c r="B276" t="n">
+        <v>241</v>
+      </c>
+      <c r="C276" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D276" t="inlineStr">
+        <is>
+          <t>Jacksonville</t>
+        </is>
+      </c>
+      <c r="E276" t="n">
+        <v>6</v>
+      </c>
+      <c r="F276" t="n">
+        <v>3</v>
+      </c>
+      <c r="G276" t="n">
+        <v>0</v>
+      </c>
+      <c r="H276" t="n">
+        <v>8</v>
+      </c>
+      <c r="I276" t="n">
+        <v>17</v>
+      </c>
+      <c r="J276" t="n">
+        <v>48</v>
+      </c>
+      <c r="K276" t="n">
+        <v>48</v>
+      </c>
+      <c r="L276" t="n">
+        <v>350</v>
+      </c>
+      <c r="M276" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="n">
+        <v>1114</v>
+      </c>
+      <c r="B277" t="n">
+        <v>242</v>
+      </c>
+      <c r="C277" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D277" t="inlineStr">
+        <is>
+          <t>Indianapolis</t>
+        </is>
+      </c>
+      <c r="E277" t="n">
+        <v>17</v>
+      </c>
+      <c r="F277" t="n">
+        <v>3</v>
+      </c>
+      <c r="G277" t="n">
+        <v>0</v>
+      </c>
+      <c r="H277" t="n">
+        <v>3</v>
+      </c>
+      <c r="I277" t="n">
+        <v>23</v>
+      </c>
+      <c r="J277" t="n">
+        <v>-10.5</v>
+      </c>
+      <c r="K277" t="n">
+        <v>11.5</v>
+      </c>
+      <c r="L277" t="n">
+        <v>-420</v>
+      </c>
+      <c r="M277" t="n">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" t="n">
+        <v>1114</v>
+      </c>
+      <c r="B278" t="n">
+        <v>243</v>
+      </c>
+      <c r="C278" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D278" t="inlineStr">
+        <is>
+          <t>Cleveland</t>
+        </is>
+      </c>
+      <c r="E278" t="n">
+        <v>7</v>
+      </c>
+      <c r="F278" t="n">
+        <v>0</v>
+      </c>
+      <c r="G278" t="n">
+        <v>0</v>
+      </c>
+      <c r="H278" t="n">
+        <v>0</v>
+      </c>
+      <c r="I278" t="n">
+        <v>7</v>
+      </c>
+      <c r="J278" t="n">
+        <v>44.5</v>
+      </c>
+      <c r="K278" t="n">
+        <v>44.5</v>
+      </c>
+      <c r="L278" t="n">
+        <v>125</v>
+      </c>
+      <c r="M278" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" t="n">
+        <v>1114</v>
+      </c>
+      <c r="B279" t="n">
+        <v>244</v>
+      </c>
+      <c r="C279" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D279" t="inlineStr">
+        <is>
+          <t>NewEngland</t>
+        </is>
+      </c>
+      <c r="E279" t="n">
+        <v>7</v>
+      </c>
+      <c r="F279" t="n">
+        <v>17</v>
+      </c>
+      <c r="G279" t="n">
+        <v>7</v>
+      </c>
+      <c r="H279" t="n">
+        <v>14</v>
+      </c>
+      <c r="I279" t="n">
+        <v>45</v>
+      </c>
+      <c r="J279" t="n">
+        <v>-3</v>
+      </c>
+      <c r="K279" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="L279" t="n">
+        <v>-145</v>
+      </c>
+      <c r="M279" t="n">
+        <v>21.5</v>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" t="n">
+        <v>1114</v>
+      </c>
+      <c r="B280" t="n">
+        <v>245</v>
+      </c>
+      <c r="C280" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D280" t="inlineStr">
+        <is>
+          <t>Atlanta</t>
+        </is>
+      </c>
+      <c r="E280" t="n">
+        <v>3</v>
+      </c>
+      <c r="F280" t="n">
+        <v>0</v>
+      </c>
+      <c r="G280" t="n">
+        <v>0</v>
+      </c>
+      <c r="H280" t="n">
+        <v>0</v>
+      </c>
+      <c r="I280" t="n">
+        <v>3</v>
+      </c>
+      <c r="J280" t="n">
+        <v>51.5</v>
+      </c>
+      <c r="K280" t="n">
+        <v>55.5</v>
+      </c>
+      <c r="L280" t="n">
+        <v>300</v>
+      </c>
+      <c r="M280" t="n">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" t="n">
+        <v>1114</v>
+      </c>
+      <c r="B281" t="n">
+        <v>246</v>
+      </c>
+      <c r="C281" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D281" t="inlineStr">
+        <is>
+          <t>Dallas</t>
+        </is>
+      </c>
+      <c r="E281" t="n">
+        <v>7</v>
+      </c>
+      <c r="F281" t="n">
+        <v>29</v>
+      </c>
+      <c r="G281" t="n">
+        <v>7</v>
+      </c>
+      <c r="H281" t="n">
+        <v>0</v>
+      </c>
+      <c r="I281" t="n">
+        <v>43</v>
+      </c>
+      <c r="J281" t="n">
+        <v>-9.5</v>
+      </c>
+      <c r="K281" t="n">
+        <v>9</v>
+      </c>
+      <c r="L281" t="n">
+        <v>-360</v>
+      </c>
+      <c r="M281" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" t="n">
+        <v>1114</v>
+      </c>
+      <c r="B282" t="n">
+        <v>247</v>
+      </c>
+      <c r="C282" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D282" t="inlineStr">
+        <is>
+          <t>Buffalo</t>
+        </is>
+      </c>
+      <c r="E282" t="n">
+        <v>10</v>
+      </c>
+      <c r="F282" t="n">
+        <v>7</v>
+      </c>
+      <c r="G282" t="n">
+        <v>21</v>
+      </c>
+      <c r="H282" t="n">
+        <v>7</v>
+      </c>
+      <c r="I282" t="n">
+        <v>45</v>
+      </c>
+      <c r="J282" t="n">
+        <v>-13.5</v>
+      </c>
+      <c r="K282" t="n">
+        <v>14</v>
+      </c>
+      <c r="L282" t="n">
+        <v>-800</v>
+      </c>
+      <c r="M282" t="n">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" t="n">
+        <v>1114</v>
+      </c>
+      <c r="B283" t="n">
+        <v>248</v>
+      </c>
+      <c r="C283" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D283" t="inlineStr">
+        <is>
+          <t>NYJets</t>
+        </is>
+      </c>
+      <c r="E283" t="n">
+        <v>0</v>
+      </c>
+      <c r="F283" t="n">
+        <v>3</v>
+      </c>
+      <c r="G283" t="n">
+        <v>0</v>
+      </c>
+      <c r="H283" t="n">
+        <v>14</v>
+      </c>
+      <c r="I283" t="n">
+        <v>17</v>
+      </c>
+      <c r="J283" t="n">
+        <v>48.5</v>
+      </c>
+      <c r="K283" t="n">
+        <v>48.5</v>
+      </c>
+      <c r="L283" t="n">
+        <v>550</v>
+      </c>
+      <c r="M283" t="n">
+        <v>21.5</v>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" t="n">
+        <v>1114</v>
+      </c>
+      <c r="B284" t="n">
+        <v>249</v>
+      </c>
+      <c r="C284" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D284" t="inlineStr">
+        <is>
+          <t>NewOrleans</t>
+        </is>
+      </c>
+      <c r="E284" t="n">
+        <v>0</v>
+      </c>
+      <c r="F284" t="n">
+        <v>6</v>
+      </c>
+      <c r="G284" t="n">
+        <v>6</v>
+      </c>
+      <c r="H284" t="n">
+        <v>9</v>
+      </c>
+      <c r="I284" t="n">
+        <v>21</v>
+      </c>
+      <c r="J284" t="n">
+        <v>44.5</v>
+      </c>
+      <c r="K284" t="n">
+        <v>42.5</v>
+      </c>
+      <c r="L284" t="n">
+        <v>130</v>
+      </c>
+      <c r="M284" t="n">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" t="n">
+        <v>1114</v>
+      </c>
+      <c r="B285" t="n">
+        <v>250</v>
+      </c>
+      <c r="C285" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D285" t="inlineStr">
+        <is>
+          <t>Tennessee</t>
+        </is>
+      </c>
+      <c r="E285" t="n">
+        <v>3</v>
+      </c>
+      <c r="F285" t="n">
+        <v>10</v>
+      </c>
+      <c r="G285" t="n">
+        <v>7</v>
+      </c>
+      <c r="H285" t="n">
+        <v>3</v>
+      </c>
+      <c r="I285" t="n">
+        <v>23</v>
+      </c>
+      <c r="J285" t="n">
+        <v>-2.5</v>
+      </c>
+      <c r="K285" t="n">
+        <v>3</v>
+      </c>
+      <c r="L285" t="n">
+        <v>-150</v>
+      </c>
+      <c r="M285" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" t="n">
+        <v>1114</v>
+      </c>
+      <c r="B286" t="n">
+        <v>251</v>
+      </c>
+      <c r="C286" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D286" t="inlineStr">
+        <is>
+          <t>TampaBay</t>
+        </is>
+      </c>
+      <c r="E286" t="n">
+        <v>0</v>
+      </c>
+      <c r="F286" t="n">
+        <v>6</v>
+      </c>
+      <c r="G286" t="n">
+        <v>7</v>
+      </c>
+      <c r="H286" t="n">
+        <v>6</v>
+      </c>
+      <c r="I286" t="n">
+        <v>19</v>
+      </c>
+      <c r="J286" t="n">
+        <v>-8</v>
+      </c>
+      <c r="K286" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="L286" t="n">
+        <v>-430</v>
+      </c>
+      <c r="M286" t="n">
+        <v>-7.5</v>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" t="n">
+        <v>1114</v>
+      </c>
+      <c r="B287" t="n">
+        <v>252</v>
+      </c>
+      <c r="C287" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D287" t="inlineStr">
+        <is>
+          <t>Washington</t>
+        </is>
+      </c>
+      <c r="E287" t="n">
+        <v>6</v>
+      </c>
+      <c r="F287" t="n">
+        <v>10</v>
+      </c>
+      <c r="G287" t="n">
+        <v>7</v>
+      </c>
+      <c r="H287" t="n">
+        <v>6</v>
+      </c>
+      <c r="I287" t="n">
+        <v>29</v>
+      </c>
+      <c r="J287" t="n">
+        <v>51</v>
+      </c>
+      <c r="K287" t="n">
+        <v>51</v>
+      </c>
+      <c r="L287" t="n">
+        <v>360</v>
+      </c>
+      <c r="M287" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" t="n">
+        <v>1114</v>
+      </c>
+      <c r="B288" t="n">
+        <v>253</v>
+      </c>
+      <c r="C288" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D288" t="inlineStr">
+        <is>
+          <t>Detroit</t>
+        </is>
+      </c>
+      <c r="E288" t="n">
+        <v>0</v>
+      </c>
+      <c r="F288" t="n">
+        <v>10</v>
+      </c>
+      <c r="G288" t="n">
+        <v>6</v>
+      </c>
+      <c r="H288" t="n">
+        <v>0</v>
+      </c>
+      <c r="I288" t="n">
+        <v>16</v>
+      </c>
+      <c r="J288" t="n">
+        <v>44</v>
+      </c>
+      <c r="K288" t="n">
+        <v>40.5</v>
+      </c>
+      <c r="L288" t="n">
+        <v>210</v>
+      </c>
+      <c r="M288" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" t="n">
+        <v>1114</v>
+      </c>
+      <c r="B289" t="n">
+        <v>254</v>
+      </c>
+      <c r="C289" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D289" t="inlineStr">
+        <is>
+          <t>Pittsburgh</t>
+        </is>
+      </c>
+      <c r="E289" t="n">
+        <v>7</v>
+      </c>
+      <c r="F289" t="n">
+        <v>3</v>
+      </c>
+      <c r="G289" t="n">
+        <v>3</v>
+      </c>
+      <c r="H289" t="n">
+        <v>3</v>
+      </c>
+      <c r="I289" t="n">
+        <v>16</v>
+      </c>
+      <c r="J289" t="n">
+        <v>-9</v>
+      </c>
+      <c r="K289" t="n">
+        <v>-6</v>
+      </c>
+      <c r="L289" t="n">
+        <v>-250</v>
+      </c>
+      <c r="M289" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" t="n">
+        <v>1114</v>
+      </c>
+      <c r="B290" t="n">
+        <v>255</v>
+      </c>
+      <c r="C290" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D290" t="inlineStr">
+        <is>
+          <t>Minnesota</t>
+        </is>
+      </c>
+      <c r="E290" t="n">
+        <v>0</v>
+      </c>
+      <c r="F290" t="n">
+        <v>13</v>
+      </c>
+      <c r="G290" t="n">
+        <v>7</v>
+      </c>
+      <c r="H290" t="n">
+        <v>7</v>
+      </c>
+      <c r="I290" t="n">
+        <v>27</v>
+      </c>
+      <c r="J290" t="n">
+        <v>50.5</v>
+      </c>
+      <c r="K290" t="n">
+        <v>53.5</v>
+      </c>
+      <c r="L290" t="n">
+        <v>155</v>
+      </c>
+      <c r="M290" t="n">
+        <v>26.5</v>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" t="n">
+        <v>1114</v>
+      </c>
+      <c r="B291" t="n">
+        <v>256</v>
+      </c>
+      <c r="C291" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D291" t="inlineStr">
+        <is>
+          <t>LAChargers</t>
+        </is>
+      </c>
+      <c r="E291" t="n">
+        <v>0</v>
+      </c>
+      <c r="F291" t="n">
+        <v>10</v>
+      </c>
+      <c r="G291" t="n">
+        <v>7</v>
+      </c>
+      <c r="H291" t="n">
+        <v>3</v>
+      </c>
+      <c r="I291" t="n">
+        <v>20</v>
+      </c>
+      <c r="J291" t="n">
+        <v>3</v>
+      </c>
+      <c r="K291" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="L291" t="n">
+        <v>-175</v>
+      </c>
+      <c r="M291" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" t="n">
+        <v>1114</v>
+      </c>
+      <c r="B292" t="n">
+        <v>257</v>
+      </c>
+      <c r="C292" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D292" t="inlineStr">
+        <is>
+          <t>Carolina</t>
+        </is>
+      </c>
+      <c r="E292" t="n">
+        <v>17</v>
+      </c>
+      <c r="F292" t="n">
+        <v>6</v>
+      </c>
+      <c r="G292" t="n">
+        <v>8</v>
+      </c>
+      <c r="H292" t="n">
+        <v>3</v>
+      </c>
+      <c r="I292" t="n">
+        <v>34</v>
+      </c>
+      <c r="J292" t="n">
+        <v>45.5</v>
+      </c>
+      <c r="K292" t="n">
+        <v>41.5</v>
+      </c>
+      <c r="L292" t="n">
+        <v>270</v>
+      </c>
+      <c r="M292" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" t="n">
+        <v>1114</v>
+      </c>
+      <c r="B293" t="n">
+        <v>258</v>
+      </c>
+      <c r="C293" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D293" t="inlineStr">
+        <is>
+          <t>Arizona</t>
+        </is>
+      </c>
+      <c r="E293" t="n">
+        <v>0</v>
+      </c>
+      <c r="F293" t="n">
+        <v>0</v>
+      </c>
+      <c r="G293" t="n">
+        <v>3</v>
+      </c>
+      <c r="H293" t="n">
+        <v>7</v>
+      </c>
+      <c r="I293" t="n">
+        <v>10</v>
+      </c>
+      <c r="J293" t="n">
+        <v>11.5</v>
+      </c>
+      <c r="K293" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="L293" t="n">
+        <v>-330</v>
+      </c>
+      <c r="M293" t="n">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" t="n">
+        <v>1114</v>
+      </c>
+      <c r="B294" t="n">
+        <v>259</v>
+      </c>
+      <c r="C294" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D294" t="inlineStr">
+        <is>
+          <t>Seattle</t>
+        </is>
+      </c>
+      <c r="E294" t="n">
+        <v>0</v>
+      </c>
+      <c r="F294" t="n">
+        <v>0</v>
+      </c>
+      <c r="G294" t="n">
+        <v>0</v>
+      </c>
+      <c r="H294" t="n">
+        <v>0</v>
+      </c>
+      <c r="I294" t="n">
+        <v>0</v>
+      </c>
+      <c r="J294" t="n">
+        <v>49.5</v>
+      </c>
+      <c r="K294" t="n">
+        <v>49</v>
+      </c>
+      <c r="L294" t="n">
+        <v>145</v>
+      </c>
+      <c r="M294" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" t="n">
+        <v>1114</v>
+      </c>
+      <c r="B295" t="n">
+        <v>260</v>
+      </c>
+      <c r="C295" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D295" t="inlineStr">
+        <is>
+          <t>GreenBay</t>
+        </is>
+      </c>
+      <c r="E295" t="n">
+        <v>0</v>
+      </c>
+      <c r="F295" t="n">
+        <v>3</v>
+      </c>
+      <c r="G295" t="n">
+        <v>0</v>
+      </c>
+      <c r="H295" t="n">
+        <v>14</v>
+      </c>
+      <c r="I295" t="n">
+        <v>17</v>
+      </c>
+      <c r="J295" t="n">
+        <v>-6</v>
+      </c>
+      <c r="K295" t="n">
+        <v>3</v>
+      </c>
+      <c r="L295" t="n">
+        <v>-165</v>
+      </c>
+      <c r="M295" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" t="n">
+        <v>1114</v>
+      </c>
+      <c r="B296" t="n">
+        <v>261</v>
+      </c>
+      <c r="C296" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D296" t="inlineStr">
+        <is>
+          <t>Philadelphia</t>
+        </is>
+      </c>
+      <c r="E296" t="n">
+        <v>10</v>
+      </c>
+      <c r="F296" t="n">
+        <v>10</v>
+      </c>
+      <c r="G296" t="n">
+        <v>7</v>
+      </c>
+      <c r="H296" t="n">
+        <v>3</v>
+      </c>
+      <c r="I296" t="n">
+        <v>30</v>
+      </c>
+      <c r="J296" t="n">
+        <v>44.5</v>
+      </c>
+      <c r="K296" t="n">
+        <v>44.5</v>
+      </c>
+      <c r="L296" t="n">
+        <v>-105</v>
+      </c>
+      <c r="M296" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" t="n">
+        <v>1114</v>
+      </c>
+      <c r="B297" t="n">
+        <v>262</v>
+      </c>
+      <c r="C297" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D297" t="inlineStr">
+        <is>
+          <t>Denver</t>
+        </is>
+      </c>
+      <c r="E297" t="n">
+        <v>0</v>
+      </c>
+      <c r="F297" t="n">
+        <v>10</v>
+      </c>
+      <c r="G297" t="n">
+        <v>3</v>
+      </c>
+      <c r="H297" t="n">
+        <v>0</v>
+      </c>
+      <c r="I297" t="n">
+        <v>13</v>
+      </c>
+      <c r="J297" t="n">
+        <v>-1.5</v>
+      </c>
+      <c r="K297" t="inlineStr">
+        <is>
+          <t>pk</t>
+        </is>
+      </c>
+      <c r="L297" t="n">
+        <v>-115</v>
+      </c>
+      <c r="M297" t="n">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" t="n">
+        <v>1114</v>
+      </c>
+      <c r="B298" t="n">
+        <v>263</v>
+      </c>
+      <c r="C298" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D298" t="inlineStr">
+        <is>
+          <t>KansasCity</t>
+        </is>
+      </c>
+      <c r="E298" t="n">
+        <v>7</v>
+      </c>
+      <c r="F298" t="n">
+        <v>10</v>
+      </c>
+      <c r="G298" t="n">
+        <v>10</v>
+      </c>
+      <c r="H298" t="n">
+        <v>14</v>
+      </c>
+      <c r="I298" t="n">
+        <v>41</v>
+      </c>
+      <c r="J298" t="n">
+        <v>-3</v>
+      </c>
+      <c r="K298" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="L298" t="n">
+        <v>-145</v>
+      </c>
+      <c r="M298" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" t="n">
+        <v>1114</v>
+      </c>
+      <c r="B299" t="n">
+        <v>264</v>
+      </c>
+      <c r="C299" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D299" t="inlineStr">
+        <is>
+          <t>LasVegas</t>
+        </is>
+      </c>
+      <c r="E299" t="n">
+        <v>0</v>
+      </c>
+      <c r="F299" t="n">
+        <v>7</v>
+      </c>
+      <c r="G299" t="n">
+        <v>7</v>
+      </c>
+      <c r="H299" t="n">
+        <v>0</v>
+      </c>
+      <c r="I299" t="n">
+        <v>14</v>
+      </c>
+      <c r="J299" t="n">
+        <v>53.5</v>
+      </c>
+      <c r="K299" t="n">
+        <v>53.5</v>
+      </c>
+      <c r="L299" t="n">
+        <v>125</v>
+      </c>
+      <c r="M299" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" t="n">
+        <v>1115</v>
+      </c>
+      <c r="B300" t="n">
+        <v>265</v>
+      </c>
+      <c r="C300" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D300" t="inlineStr">
+        <is>
+          <t>LARams</t>
+        </is>
+      </c>
+      <c r="E300" t="n">
+        <v>0</v>
+      </c>
+      <c r="F300" t="n">
+        <v>7</v>
+      </c>
+      <c r="G300" t="n">
+        <v>0</v>
+      </c>
+      <c r="H300" t="n">
+        <v>3</v>
+      </c>
+      <c r="I300" t="n">
+        <v>10</v>
+      </c>
+      <c r="J300" t="n">
+        <v>3</v>
+      </c>
+      <c r="K300" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="L300" t="n">
+        <v>-190</v>
+      </c>
+      <c r="M300" t="n">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" t="n">
+        <v>1115</v>
+      </c>
+      <c r="B301" t="n">
+        <v>266</v>
+      </c>
+      <c r="C301" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="D301" t="inlineStr">
+        <is>
+          <t>SanFrancisco</t>
+        </is>
+      </c>
+      <c r="E301" t="n">
+        <v>14</v>
+      </c>
+      <c r="F301" t="n">
+        <v>7</v>
+      </c>
+      <c r="G301" t="n">
+        <v>3</v>
+      </c>
+      <c r="H301" t="n">
+        <v>7</v>
+      </c>
+      <c r="I301" t="n">
+        <v>31</v>
+      </c>
+      <c r="J301" t="n">
+        <v>47</v>
+      </c>
+      <c r="K301" t="n">
+        <v>50</v>
+      </c>
+      <c r="L301" t="n">
+        <v>170</v>
+      </c>
+      <c r="M301" t="n">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
code working for nba
</commit_message>
<xml_diff>
--- a/Data/Odds/NFL/NFL odds 2021-22.xlsx
+++ b/Data/Odds/NFL/NFL odds 2021-22.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -50,6 +50,7 @@
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">

</xml_diff>